<commit_message>
Laadprijzen toegevoegd aan rusttijdstippen
* In app: laadprijzen toegevoegd
* Excel met prijzen toegevoegd
* Testscript voor lokaal laadmodel toegevoegd
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin Buijs\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin Buijs\Documents\GitHub\laadmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF1C254F-34E0-49C4-81F3-300825FF164C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506D4487-038C-407A-BB5A-E2AFA2401224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -92,7 +92,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,1366 +395,1082 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>45937.916666666657</v>
       </c>
       <c r="B2" s="2">
-        <v>45937.916666666657</v>
-      </c>
-      <c r="C2" s="2">
         <v>45938</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>101.74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>45937.927083333343</v>
       </c>
       <c r="B3" s="2">
-        <v>45937.927083333343</v>
-      </c>
-      <c r="C3" s="2">
         <v>45938.010416666657</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>91.4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>45937.9375</v>
       </c>
       <c r="B4" s="2">
-        <v>45937.9375</v>
-      </c>
-      <c r="C4" s="2">
         <v>45938.020833333343</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>91.47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>45937.947916666657</v>
       </c>
       <c r="B5" s="2">
-        <v>45937.947916666657</v>
-      </c>
-      <c r="C5" s="2">
         <v>45938.03125</v>
       </c>
-      <c r="D5">
+      <c r="C5">
         <v>89.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>4</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>45937.958333333343</v>
       </c>
       <c r="B6" s="2">
-        <v>45937.958333333343</v>
-      </c>
-      <c r="C6" s="2">
         <v>45938.041666666657</v>
       </c>
-      <c r="D6">
+      <c r="C6">
         <v>91.85</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>5</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>45937.96875</v>
       </c>
       <c r="B7" s="2">
-        <v>45937.96875</v>
-      </c>
-      <c r="C7" s="2">
         <v>45938.052083333343</v>
       </c>
-      <c r="D7">
+      <c r="C7">
         <v>89.07</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>6</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>45937.979166666657</v>
       </c>
       <c r="B8" s="2">
-        <v>45937.979166666657</v>
-      </c>
-      <c r="C8" s="2">
         <v>45938.0625</v>
       </c>
-      <c r="D8">
+      <c r="C8">
         <v>87.33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>45937.989583333343</v>
       </c>
       <c r="B9" s="2">
-        <v>45937.989583333343</v>
-      </c>
-      <c r="C9" s="2">
         <v>45938.072916666657</v>
       </c>
-      <c r="D9">
+      <c r="C9">
         <v>85.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>8</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>45938</v>
       </c>
       <c r="B10" s="2">
-        <v>45938</v>
-      </c>
-      <c r="C10" s="2">
         <v>45938.083333333343</v>
       </c>
-      <c r="D10">
+      <c r="C10">
         <v>89.21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>9</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>45938.010416666657</v>
       </c>
       <c r="B11" s="2">
-        <v>45938.010416666657</v>
-      </c>
-      <c r="C11" s="2">
         <v>45938.09375</v>
       </c>
-      <c r="D11">
+      <c r="C11">
         <v>88.14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>10</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>45938.020833333343</v>
       </c>
       <c r="B12" s="2">
-        <v>45938.020833333343</v>
-      </c>
-      <c r="C12" s="2">
         <v>45938.104166666657</v>
       </c>
-      <c r="D12">
+      <c r="C12">
         <v>86.99</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>11</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>45938.03125</v>
       </c>
       <c r="B13" s="2">
-        <v>45938.03125</v>
-      </c>
-      <c r="C13" s="2">
         <v>45938.114583333343</v>
       </c>
-      <c r="D13">
+      <c r="C13">
         <v>85.9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>12</v>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>45938.041666666657</v>
       </c>
       <c r="B14" s="2">
-        <v>45938.041666666657</v>
-      </c>
-      <c r="C14" s="2">
         <v>45938.125</v>
       </c>
-      <c r="D14">
+      <c r="C14">
         <v>86.71</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>13</v>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>45938.052083333343</v>
       </c>
       <c r="B15" s="2">
-        <v>45938.052083333343</v>
-      </c>
-      <c r="C15" s="2">
         <v>45938.135416666657</v>
       </c>
-      <c r="D15">
+      <c r="C15">
         <v>84.17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>14</v>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>45938.0625</v>
       </c>
       <c r="B16" s="2">
-        <v>45938.0625</v>
-      </c>
-      <c r="C16" s="2">
         <v>45938.145833333343</v>
       </c>
-      <c r="D16">
+      <c r="C16">
         <v>86.98</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>15</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>45938.072916666657</v>
       </c>
       <c r="B17" s="2">
-        <v>45938.072916666657</v>
-      </c>
-      <c r="C17" s="2">
         <v>45938.15625</v>
       </c>
-      <c r="D17">
+      <c r="C17">
         <v>86.17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>16</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>45938.083333333343</v>
       </c>
       <c r="B18" s="2">
-        <v>45938.083333333343</v>
-      </c>
-      <c r="C18" s="2">
         <v>45938.166666666657</v>
       </c>
-      <c r="D18">
+      <c r="C18">
         <v>85.66</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>17</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>45938.09375</v>
       </c>
       <c r="B19" s="2">
-        <v>45938.09375</v>
-      </c>
-      <c r="C19" s="2">
         <v>45938.177083333343</v>
       </c>
-      <c r="D19">
+      <c r="C19">
         <v>84.48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>18</v>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>45938.104166666657</v>
       </c>
       <c r="B20" s="2">
-        <v>45938.104166666657</v>
-      </c>
-      <c r="C20" s="2">
         <v>45938.1875</v>
       </c>
-      <c r="D20">
+      <c r="C20">
         <v>87.11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>19</v>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>45938.114583333343</v>
       </c>
       <c r="B21" s="2">
-        <v>45938.114583333343</v>
-      </c>
-      <c r="C21" s="2">
         <v>45938.197916666657</v>
       </c>
-      <c r="D21">
+      <c r="C21">
         <v>91.67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>20</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>45938.125</v>
       </c>
       <c r="B22" s="2">
-        <v>45938.125</v>
-      </c>
-      <c r="C22" s="2">
         <v>45938.208333333343</v>
       </c>
-      <c r="D22">
+      <c r="C22">
         <v>86.98</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>21</v>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>45938.135416666657</v>
       </c>
       <c r="B23" s="2">
-        <v>45938.135416666657</v>
-      </c>
-      <c r="C23" s="2">
         <v>45938.21875</v>
       </c>
-      <c r="D23">
+      <c r="C23">
         <v>93.28</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>22</v>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>45938.145833333343</v>
       </c>
       <c r="B24" s="2">
-        <v>45938.145833333343</v>
-      </c>
-      <c r="C24" s="2">
         <v>45938.229166666657</v>
       </c>
-      <c r="D24">
+      <c r="C24">
         <v>92.51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>23</v>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>45938.15625</v>
       </c>
       <c r="B25" s="2">
-        <v>45938.15625</v>
-      </c>
-      <c r="C25" s="2">
         <v>45938.239583333343</v>
       </c>
-      <c r="D25">
+      <c r="C25">
         <v>102.9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>24</v>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>45938.166666666657</v>
       </c>
       <c r="B26" s="2">
-        <v>45938.166666666657</v>
-      </c>
-      <c r="C26" s="2">
         <v>45938.25</v>
       </c>
-      <c r="D26">
+      <c r="C26">
         <v>92.99</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>25</v>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>45938.177083333343</v>
       </c>
       <c r="B27" s="2">
-        <v>45938.177083333343</v>
-      </c>
-      <c r="C27" s="2">
         <v>45938.260416666657</v>
       </c>
-      <c r="D27">
+      <c r="C27">
         <v>108.63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>26</v>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>45938.1875</v>
       </c>
       <c r="B28" s="2">
-        <v>45938.1875</v>
-      </c>
-      <c r="C28" s="2">
         <v>45938.270833333343</v>
       </c>
-      <c r="D28">
+      <c r="C28">
         <v>120.42</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>27</v>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>45938.197916666657</v>
       </c>
       <c r="B29" s="2">
-        <v>45938.197916666657</v>
-      </c>
-      <c r="C29" s="2">
         <v>45938.28125</v>
       </c>
-      <c r="D29">
+      <c r="C29">
         <v>134.53</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>28</v>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>45938.208333333343</v>
       </c>
       <c r="B30" s="2">
-        <v>45938.208333333343</v>
-      </c>
-      <c r="C30" s="2">
         <v>45938.291666666657</v>
       </c>
-      <c r="D30">
+      <c r="C30">
         <v>127.56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>29</v>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>45938.21875</v>
       </c>
       <c r="B31" s="2">
-        <v>45938.21875</v>
-      </c>
-      <c r="C31" s="2">
         <v>45938.302083333343</v>
       </c>
-      <c r="D31">
+      <c r="C31">
         <v>148.38999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>30</v>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>45938.229166666657</v>
       </c>
       <c r="B32" s="2">
-        <v>45938.229166666657</v>
-      </c>
-      <c r="C32" s="2">
         <v>45938.3125</v>
       </c>
-      <c r="D32">
+      <c r="C32">
         <v>165.45</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>31</v>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>45938.239583333343</v>
       </c>
       <c r="B33" s="2">
-        <v>45938.239583333343</v>
-      </c>
-      <c r="C33" s="2">
         <v>45938.322916666657</v>
       </c>
-      <c r="D33">
+      <c r="C33">
         <v>168.83</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>32</v>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>45938.25</v>
       </c>
       <c r="B34" s="2">
-        <v>45938.25</v>
-      </c>
-      <c r="C34" s="2">
         <v>45938.333333333343</v>
       </c>
-      <c r="D34">
+      <c r="C34">
         <v>203.62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>33</v>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>45938.260416666657</v>
       </c>
       <c r="B35" s="2">
-        <v>45938.260416666657</v>
-      </c>
-      <c r="C35" s="2">
         <v>45938.34375</v>
       </c>
-      <c r="D35">
+      <c r="C35">
         <v>175.34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>34</v>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>45938.270833333343</v>
       </c>
       <c r="B36" s="2">
-        <v>45938.270833333343</v>
-      </c>
-      <c r="C36" s="2">
         <v>45938.354166666657</v>
       </c>
-      <c r="D36">
+      <c r="C36">
         <v>151.24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>35</v>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>45938.28125</v>
       </c>
       <c r="B37" s="2">
-        <v>45938.28125</v>
-      </c>
-      <c r="C37" s="2">
         <v>45938.364583333343</v>
       </c>
-      <c r="D37">
+      <c r="C37">
         <v>135.38</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>36</v>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>45938.291666666657</v>
       </c>
       <c r="B38" s="2">
-        <v>45938.291666666657</v>
-      </c>
-      <c r="C38" s="2">
         <v>45938.375</v>
       </c>
-      <c r="D38">
+      <c r="C38">
         <v>176.35</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
-        <v>37</v>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>45938.302083333343</v>
       </c>
       <c r="B39" s="2">
-        <v>45938.302083333343</v>
-      </c>
-      <c r="C39" s="2">
         <v>45938.385416666657</v>
       </c>
-      <c r="D39">
+      <c r="C39">
         <v>142.44999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
-        <v>38</v>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>45938.3125</v>
       </c>
       <c r="B40" s="2">
-        <v>45938.3125</v>
-      </c>
-      <c r="C40" s="2">
         <v>45938.395833333343</v>
       </c>
-      <c r="D40">
+      <c r="C40">
         <v>119.67</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
-        <v>39</v>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>45938.322916666657</v>
       </c>
       <c r="B41" s="2">
-        <v>45938.322916666657</v>
-      </c>
-      <c r="C41" s="2">
         <v>45938.40625</v>
       </c>
-      <c r="D41">
+      <c r="C41">
         <v>106.06</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
-        <v>40</v>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>45938.333333333343</v>
       </c>
       <c r="B42" s="2">
-        <v>45938.333333333343</v>
-      </c>
-      <c r="C42" s="2">
         <v>45938.416666666657</v>
       </c>
-      <c r="D42">
+      <c r="C42">
         <v>139.21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
-        <v>41</v>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>45938.34375</v>
       </c>
       <c r="B43" s="2">
-        <v>45938.34375</v>
-      </c>
-      <c r="C43" s="2">
         <v>45938.427083333343</v>
       </c>
-      <c r="D43">
+      <c r="C43">
         <v>119.74</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
-        <v>42</v>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>45938.354166666657</v>
       </c>
       <c r="B44" s="2">
-        <v>45938.354166666657</v>
-      </c>
-      <c r="C44" s="2">
         <v>45938.4375</v>
       </c>
-      <c r="D44">
+      <c r="C44">
         <v>106.31</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
-        <v>43</v>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>45938.364583333343</v>
       </c>
       <c r="B45" s="2">
-        <v>45938.364583333343</v>
-      </c>
-      <c r="C45" s="2">
         <v>45938.447916666657</v>
       </c>
-      <c r="D45">
+      <c r="C45">
         <v>99.46</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>44</v>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>45938.375</v>
       </c>
       <c r="B46" s="2">
-        <v>45938.375</v>
-      </c>
-      <c r="C46" s="2">
         <v>45938.458333333343</v>
       </c>
-      <c r="D46">
+      <c r="C46">
         <v>120.14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
-        <v>45</v>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>45938.385416666657</v>
       </c>
       <c r="B47" s="2">
-        <v>45938.385416666657</v>
-      </c>
-      <c r="C47" s="2">
         <v>45938.46875</v>
       </c>
-      <c r="D47">
+      <c r="C47">
         <v>101.96</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
-        <v>46</v>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>45938.395833333343</v>
       </c>
       <c r="B48" s="2">
-        <v>45938.395833333343</v>
-      </c>
-      <c r="C48" s="2">
         <v>45938.479166666657</v>
       </c>
-      <c r="D48">
+      <c r="C48">
         <v>94.05</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
-        <v>47</v>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>45938.40625</v>
       </c>
       <c r="B49" s="2">
-        <v>45938.40625</v>
-      </c>
-      <c r="C49" s="2">
         <v>45938.489583333343</v>
       </c>
-      <c r="D49">
+      <c r="C49">
         <v>85.06</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
-        <v>48</v>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>45938.416666666657</v>
       </c>
       <c r="B50" s="2">
-        <v>45938.416666666657</v>
-      </c>
-      <c r="C50" s="2">
         <v>45938.5</v>
       </c>
-      <c r="D50">
+      <c r="C50">
         <v>92.65</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
-        <v>49</v>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>45938.427083333343</v>
       </c>
       <c r="B51" s="2">
-        <v>45938.427083333343</v>
-      </c>
-      <c r="C51" s="2">
         <v>45938.510416666657</v>
       </c>
-      <c r="D51">
+      <c r="C51">
         <v>88.73</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
-        <v>50</v>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>45938.4375</v>
       </c>
       <c r="B52" s="2">
-        <v>45938.4375</v>
-      </c>
-      <c r="C52" s="2">
         <v>45938.520833333343</v>
       </c>
-      <c r="D52">
+      <c r="C52">
         <v>86.6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="1">
-        <v>51</v>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>45938.447916666657</v>
       </c>
       <c r="B53" s="2">
-        <v>45938.447916666657</v>
-      </c>
-      <c r="C53" s="2">
         <v>45938.53125</v>
       </c>
-      <c r="D53">
+      <c r="C53">
         <v>86.05</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="1">
-        <v>52</v>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>45938.458333333343</v>
       </c>
       <c r="B54" s="2">
-        <v>45938.458333333343</v>
-      </c>
-      <c r="C54" s="2">
         <v>45938.541666666657</v>
       </c>
-      <c r="D54">
+      <c r="C54">
         <v>88.93</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="1">
-        <v>53</v>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="2">
+        <v>45938.46875</v>
       </c>
       <c r="B55" s="2">
-        <v>45938.46875</v>
-      </c>
-      <c r="C55" s="2">
         <v>45938.552083333343</v>
       </c>
-      <c r="D55">
+      <c r="C55">
         <v>87.74</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="1">
-        <v>54</v>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="2">
+        <v>45938.479166666657</v>
       </c>
       <c r="B56" s="2">
-        <v>45938.479166666657</v>
-      </c>
-      <c r="C56" s="2">
         <v>45938.5625</v>
       </c>
-      <c r="D56">
+      <c r="C56">
         <v>86.06</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="1">
-        <v>55</v>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="2">
+        <v>45938.489583333343</v>
       </c>
       <c r="B57" s="2">
-        <v>45938.489583333343</v>
-      </c>
-      <c r="C57" s="2">
         <v>45938.572916666657</v>
       </c>
-      <c r="D57">
+      <c r="C57">
         <v>84.38</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="1">
-        <v>56</v>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="2">
+        <v>45938.5</v>
       </c>
       <c r="B58" s="2">
-        <v>45938.5</v>
-      </c>
-      <c r="C58" s="2">
         <v>45938.583333333343</v>
       </c>
-      <c r="D58">
+      <c r="C58">
         <v>82.93</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="1">
-        <v>57</v>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="2">
+        <v>45938.510416666657</v>
       </c>
       <c r="B59" s="2">
-        <v>45938.510416666657</v>
-      </c>
-      <c r="C59" s="2">
         <v>45938.59375</v>
       </c>
-      <c r="D59">
+      <c r="C59">
         <v>84.88</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="1">
-        <v>58</v>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="2">
+        <v>45938.520833333343</v>
       </c>
       <c r="B60" s="2">
-        <v>45938.520833333343</v>
-      </c>
-      <c r="C60" s="2">
         <v>45938.604166666657</v>
       </c>
-      <c r="D60">
+      <c r="C60">
         <v>86.66</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="1">
-        <v>59</v>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="2">
+        <v>45938.53125</v>
       </c>
       <c r="B61" s="2">
-        <v>45938.53125</v>
-      </c>
-      <c r="C61" s="2">
         <v>45938.614583333343</v>
       </c>
-      <c r="D61">
+      <c r="C61">
         <v>94.46</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="1">
-        <v>60</v>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="2">
+        <v>45938.541666666657</v>
       </c>
       <c r="B62" s="2">
-        <v>45938.541666666657</v>
-      </c>
-      <c r="C62" s="2">
         <v>45938.625</v>
       </c>
-      <c r="D62">
+      <c r="C62">
         <v>84.27</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="1">
-        <v>61</v>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="2">
+        <v>45938.552083333343</v>
       </c>
       <c r="B63" s="2">
-        <v>45938.552083333343</v>
-      </c>
-      <c r="C63" s="2">
         <v>45938.635416666657</v>
       </c>
-      <c r="D63">
+      <c r="C63">
         <v>88.51</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="1">
-        <v>62</v>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="2">
+        <v>45938.5625</v>
       </c>
       <c r="B64" s="2">
-        <v>45938.5625</v>
-      </c>
-      <c r="C64" s="2">
         <v>45938.645833333343</v>
       </c>
-      <c r="D64">
+      <c r="C64">
         <v>95.9</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="1">
-        <v>63</v>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="2">
+        <v>45938.572916666657</v>
       </c>
       <c r="B65" s="2">
-        <v>45938.572916666657</v>
-      </c>
-      <c r="C65" s="2">
         <v>45938.65625</v>
       </c>
-      <c r="D65">
+      <c r="C65">
         <v>108.61</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="1">
-        <v>64</v>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="2">
+        <v>45938.583333333343</v>
       </c>
       <c r="B66" s="2">
-        <v>45938.583333333343</v>
-      </c>
-      <c r="C66" s="2">
         <v>45938.666666666657</v>
       </c>
-      <c r="D66">
+      <c r="C66">
         <v>86.02</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="1">
-        <v>65</v>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="2">
+        <v>45938.59375</v>
       </c>
       <c r="B67" s="2">
-        <v>45938.59375</v>
-      </c>
-      <c r="C67" s="2">
         <v>45938.677083333343</v>
       </c>
-      <c r="D67">
+      <c r="C67">
         <v>94.17</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="1">
-        <v>66</v>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="2">
+        <v>45938.604166666657</v>
       </c>
       <c r="B68" s="2">
-        <v>45938.604166666657</v>
-      </c>
-      <c r="C68" s="2">
         <v>45938.6875</v>
       </c>
-      <c r="D68">
+      <c r="C68">
         <v>118.25</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="1">
-        <v>67</v>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="2">
+        <v>45938.614583333343</v>
       </c>
       <c r="B69" s="2">
-        <v>45938.614583333343</v>
-      </c>
-      <c r="C69" s="2">
         <v>45938.697916666657</v>
       </c>
-      <c r="D69">
+      <c r="C69">
         <v>139.62</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="1">
-        <v>68</v>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="2">
+        <v>45938.625</v>
       </c>
       <c r="B70" s="2">
-        <v>45938.625</v>
-      </c>
-      <c r="C70" s="2">
         <v>45938.708333333343</v>
       </c>
-      <c r="D70">
+      <c r="C70">
         <v>96.65</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="1">
-        <v>69</v>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="2">
+        <v>45938.635416666657</v>
       </c>
       <c r="B71" s="2">
-        <v>45938.635416666657</v>
-      </c>
-      <c r="C71" s="2">
         <v>45938.71875</v>
       </c>
-      <c r="D71">
+      <c r="C71">
         <v>117.95</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="1">
-        <v>70</v>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="2">
+        <v>45938.645833333343</v>
       </c>
       <c r="B72" s="2">
-        <v>45938.645833333343</v>
-      </c>
-      <c r="C72" s="2">
         <v>45938.729166666657</v>
       </c>
-      <c r="D72">
+      <c r="C72">
         <v>148.81</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" s="1">
-        <v>71</v>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="2">
+        <v>45938.65625</v>
       </c>
       <c r="B73" s="2">
-        <v>45938.65625</v>
-      </c>
-      <c r="C73" s="2">
         <v>45938.739583333343</v>
       </c>
-      <c r="D73">
+      <c r="C73">
         <v>203.12</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" s="1">
-        <v>72</v>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="2">
+        <v>45938.666666666657</v>
       </c>
       <c r="B74" s="2">
-        <v>45938.666666666657</v>
-      </c>
-      <c r="C74" s="2">
         <v>45938.75</v>
       </c>
-      <c r="D74">
+      <c r="C74">
         <v>129.74</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="1">
-        <v>73</v>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="2">
+        <v>45938.677083333343</v>
       </c>
       <c r="B75" s="2">
-        <v>45938.677083333343</v>
-      </c>
-      <c r="C75" s="2">
         <v>45938.760416666657</v>
       </c>
-      <c r="D75">
+      <c r="C75">
         <v>142.25</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="1">
-        <v>74</v>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="2">
+        <v>45938.6875</v>
       </c>
       <c r="B76" s="2">
-        <v>45938.6875</v>
-      </c>
-      <c r="C76" s="2">
         <v>45938.770833333343</v>
       </c>
-      <c r="D76">
+      <c r="C76">
         <v>195.41</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="1">
-        <v>75</v>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="2">
+        <v>45938.697916666657</v>
       </c>
       <c r="B77" s="2">
-        <v>45938.697916666657</v>
-      </c>
-      <c r="C77" s="2">
         <v>45938.78125</v>
       </c>
-      <c r="D77">
+      <c r="C77">
         <v>241.07</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="1">
-        <v>76</v>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="2">
+        <v>45938.708333333343</v>
       </c>
       <c r="B78" s="2">
-        <v>45938.708333333343</v>
-      </c>
-      <c r="C78" s="2">
         <v>45938.791666666657</v>
       </c>
-      <c r="D78">
+      <c r="C78">
         <v>223.55</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="1">
-        <v>77</v>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="2">
+        <v>45938.71875</v>
       </c>
       <c r="B79" s="2">
-        <v>45938.71875</v>
-      </c>
-      <c r="C79" s="2">
         <v>45938.802083333343</v>
       </c>
-      <c r="D79">
+      <c r="C79">
         <v>199.54</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" s="1">
-        <v>78</v>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="2">
+        <v>45938.729166666657</v>
       </c>
       <c r="B80" s="2">
-        <v>45938.729166666657</v>
-      </c>
-      <c r="C80" s="2">
         <v>45938.8125</v>
       </c>
-      <c r="D80">
+      <c r="C80">
         <v>180.46</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="1">
-        <v>79</v>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="2">
+        <v>45938.739583333343</v>
       </c>
       <c r="B81" s="2">
-        <v>45938.739583333343</v>
-      </c>
-      <c r="C81" s="2">
         <v>45938.822916666657</v>
       </c>
-      <c r="D81">
+      <c r="C81">
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="1">
-        <v>80</v>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="2">
+        <v>45938.75</v>
       </c>
       <c r="B82" s="2">
-        <v>45938.75</v>
-      </c>
-      <c r="C82" s="2">
         <v>45938.833333333343</v>
       </c>
-      <c r="D82">
+      <c r="C82">
         <v>169.2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="1">
-        <v>81</v>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="2">
+        <v>45938.760416666657</v>
       </c>
       <c r="B83" s="2">
-        <v>45938.760416666657</v>
-      </c>
-      <c r="C83" s="2">
         <v>45938.84375</v>
       </c>
-      <c r="D83">
+      <c r="C83">
         <v>149.99</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" s="1">
-        <v>82</v>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="2">
+        <v>45938.770833333343</v>
       </c>
       <c r="B84" s="2">
-        <v>45938.770833333343</v>
-      </c>
-      <c r="C84" s="2">
         <v>45938.854166666657</v>
       </c>
-      <c r="D84">
+      <c r="C84">
         <v>128.21</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A85" s="1">
-        <v>83</v>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="2">
+        <v>45938.78125</v>
       </c>
       <c r="B85" s="2">
-        <v>45938.78125</v>
-      </c>
-      <c r="C85" s="2">
         <v>45938.864583333343</v>
       </c>
-      <c r="D85">
+      <c r="C85">
         <v>118.39</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A86" s="1">
-        <v>84</v>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="2">
+        <v>45938.791666666657</v>
       </c>
       <c r="B86" s="2">
-        <v>45938.791666666657</v>
-      </c>
-      <c r="C86" s="2">
         <v>45938.875</v>
       </c>
-      <c r="D86">
+      <c r="C86">
         <v>128.02000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" s="1">
-        <v>85</v>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="2">
+        <v>45938.802083333343</v>
       </c>
       <c r="B87" s="2">
-        <v>45938.802083333343</v>
-      </c>
-      <c r="C87" s="2">
         <v>45938.885416666657</v>
       </c>
-      <c r="D87">
+      <c r="C87">
         <v>116.99</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" s="1">
-        <v>86</v>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="2">
+        <v>45938.8125</v>
       </c>
       <c r="B88" s="2">
-        <v>45938.8125</v>
-      </c>
-      <c r="C88" s="2">
         <v>45938.895833333343</v>
       </c>
-      <c r="D88">
+      <c r="C88">
         <v>106.9</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" s="1">
-        <v>87</v>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="2">
+        <v>45938.822916666657</v>
       </c>
       <c r="B89" s="2">
-        <v>45938.822916666657</v>
-      </c>
-      <c r="C89" s="2">
         <v>45938.90625</v>
       </c>
-      <c r="D89">
+      <c r="C89">
         <v>102.34</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A90" s="1">
-        <v>88</v>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="2">
+        <v>45938.833333333343</v>
       </c>
       <c r="B90" s="2">
-        <v>45938.833333333343</v>
-      </c>
-      <c r="C90" s="2">
         <v>45938.916666666657</v>
       </c>
-      <c r="D90">
+      <c r="C90">
         <v>110.69</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" s="1">
-        <v>89</v>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="2">
+        <v>45938.84375</v>
       </c>
       <c r="B91" s="2">
-        <v>45938.84375</v>
-      </c>
-      <c r="C91" s="2">
         <v>45938.927083333343</v>
       </c>
-      <c r="D91">
+      <c r="C91">
         <v>109.91</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" s="1">
-        <v>90</v>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="2">
+        <v>45938.854166666657</v>
       </c>
       <c r="B92" s="2">
-        <v>45938.854166666657</v>
-      </c>
-      <c r="C92" s="2">
         <v>45938.9375</v>
       </c>
-      <c r="D92">
+      <c r="C92">
         <v>106.28</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" s="1">
-        <v>91</v>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="2">
+        <v>45938.864583333343</v>
       </c>
       <c r="B93" s="2">
-        <v>45938.864583333343</v>
-      </c>
-      <c r="C93" s="2">
         <v>45938.947916666657</v>
       </c>
-      <c r="D93">
+      <c r="C93">
         <v>97.93</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A94" s="1">
-        <v>92</v>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="2">
+        <v>45938.875</v>
       </c>
       <c r="B94" s="2">
-        <v>45938.875</v>
-      </c>
-      <c r="C94" s="2">
         <v>45938.958333333343</v>
       </c>
-      <c r="D94">
+      <c r="C94">
         <v>101.68</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" s="1">
-        <v>93</v>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="2">
+        <v>45938.885416666657</v>
       </c>
       <c r="B95" s="2">
-        <v>45938.885416666657</v>
-      </c>
-      <c r="C95" s="2">
         <v>45938.96875</v>
       </c>
-      <c r="D95">
+      <c r="C95">
         <v>99.79</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" s="1">
-        <v>94</v>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="2">
+        <v>45938.895833333343</v>
       </c>
       <c r="B96" s="2">
-        <v>45938.895833333343</v>
-      </c>
-      <c r="C96" s="2">
         <v>45938.979166666657</v>
       </c>
-      <c r="D96">
+      <c r="C96">
         <v>95.48</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="1">
-        <v>95</v>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="2">
+        <v>45938.90625</v>
       </c>
       <c r="B97" s="2">
-        <v>45938.90625</v>
-      </c>
-      <c r="C97" s="2">
         <v>45938.989583333343</v>
       </c>
-      <c r="D97">
+      <c r="C97">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update XLSX via API 23-01-2026, 09:38:18
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3577"/>
+  <dimension ref="A1:C3673"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39746,6 +39746,1062 @@
         <v>91.98</v>
       </c>
     </row>
+    <row r="3578">
+      <c r="A3578" s="2" t="n">
+        <v>46043.95833333334</v>
+      </c>
+      <c r="B3578" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="C3578" t="n">
+        <v>88.03</v>
+      </c>
+    </row>
+    <row r="3579">
+      <c r="A3579" s="2" t="n">
+        <v>46043.96875</v>
+      </c>
+      <c r="B3579" s="2" t="n">
+        <v>46044.01041666666</v>
+      </c>
+      <c r="C3579" t="n">
+        <v>88.42</v>
+      </c>
+    </row>
+    <row r="3580">
+      <c r="A3580" s="2" t="n">
+        <v>46043.97916666666</v>
+      </c>
+      <c r="B3580" s="2" t="n">
+        <v>46044.02083333334</v>
+      </c>
+      <c r="C3580" t="n">
+        <v>85.73</v>
+      </c>
+    </row>
+    <row r="3581">
+      <c r="A3581" s="2" t="n">
+        <v>46043.98958333334</v>
+      </c>
+      <c r="B3581" s="2" t="n">
+        <v>46044.03125</v>
+      </c>
+      <c r="C3581" t="n">
+        <v>80.92</v>
+      </c>
+    </row>
+    <row r="3582">
+      <c r="A3582" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B3582" s="2" t="n">
+        <v>46044.04166666666</v>
+      </c>
+      <c r="C3582" t="n">
+        <v>89.89</v>
+      </c>
+    </row>
+    <row r="3583">
+      <c r="A3583" s="2" t="n">
+        <v>46044.01041666666</v>
+      </c>
+      <c r="B3583" s="2" t="n">
+        <v>46044.05208333334</v>
+      </c>
+      <c r="C3583" t="n">
+        <v>88.53</v>
+      </c>
+    </row>
+    <row r="3584">
+      <c r="A3584" s="2" t="n">
+        <v>46044.02083333334</v>
+      </c>
+      <c r="B3584" s="2" t="n">
+        <v>46044.0625</v>
+      </c>
+      <c r="C3584" t="n">
+        <v>87.72</v>
+      </c>
+    </row>
+    <row r="3585">
+      <c r="A3585" s="2" t="n">
+        <v>46044.03125</v>
+      </c>
+      <c r="B3585" s="2" t="n">
+        <v>46044.07291666666</v>
+      </c>
+      <c r="C3585" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3586">
+      <c r="A3586" s="2" t="n">
+        <v>46044.04166666666</v>
+      </c>
+      <c r="B3586" s="2" t="n">
+        <v>46044.08333333334</v>
+      </c>
+      <c r="C3586" t="n">
+        <v>90.18000000000001</v>
+      </c>
+    </row>
+    <row r="3587">
+      <c r="A3587" s="2" t="n">
+        <v>46044.05208333334</v>
+      </c>
+      <c r="B3587" s="2" t="n">
+        <v>46044.09375</v>
+      </c>
+      <c r="C3587" t="n">
+        <v>90.09</v>
+      </c>
+    </row>
+    <row r="3588">
+      <c r="A3588" s="2" t="n">
+        <v>46044.0625</v>
+      </c>
+      <c r="B3588" s="2" t="n">
+        <v>46044.10416666666</v>
+      </c>
+      <c r="C3588" t="n">
+        <v>89.98</v>
+      </c>
+    </row>
+    <row r="3589">
+      <c r="A3589" s="2" t="n">
+        <v>46044.07291666666</v>
+      </c>
+      <c r="B3589" s="2" t="n">
+        <v>46044.11458333334</v>
+      </c>
+      <c r="C3589" t="n">
+        <v>84.56999999999999</v>
+      </c>
+    </row>
+    <row r="3590">
+      <c r="A3590" s="2" t="n">
+        <v>46044.08333333334</v>
+      </c>
+      <c r="B3590" s="2" t="n">
+        <v>46044.125</v>
+      </c>
+      <c r="C3590" t="n">
+        <v>85.43000000000001</v>
+      </c>
+    </row>
+    <row r="3591">
+      <c r="A3591" s="2" t="n">
+        <v>46044.09375</v>
+      </c>
+      <c r="B3591" s="2" t="n">
+        <v>46044.13541666666</v>
+      </c>
+      <c r="C3591" t="n">
+        <v>83.65000000000001</v>
+      </c>
+    </row>
+    <row r="3592">
+      <c r="A3592" s="2" t="n">
+        <v>46044.10416666666</v>
+      </c>
+      <c r="B3592" s="2" t="n">
+        <v>46044.14583333334</v>
+      </c>
+      <c r="C3592" t="n">
+        <v>83.47</v>
+      </c>
+    </row>
+    <row r="3593">
+      <c r="A3593" s="2" t="n">
+        <v>46044.11458333334</v>
+      </c>
+      <c r="B3593" s="2" t="n">
+        <v>46044.15625</v>
+      </c>
+      <c r="C3593" t="n">
+        <v>83.81999999999999</v>
+      </c>
+    </row>
+    <row r="3594">
+      <c r="A3594" s="2" t="n">
+        <v>46044.125</v>
+      </c>
+      <c r="B3594" s="2" t="n">
+        <v>46044.16666666666</v>
+      </c>
+      <c r="C3594" t="n">
+        <v>83.86</v>
+      </c>
+    </row>
+    <row r="3595">
+      <c r="A3595" s="2" t="n">
+        <v>46044.13541666666</v>
+      </c>
+      <c r="B3595" s="2" t="n">
+        <v>46044.17708333334</v>
+      </c>
+      <c r="C3595" t="n">
+        <v>83.61</v>
+      </c>
+    </row>
+    <row r="3596">
+      <c r="A3596" s="2" t="n">
+        <v>46044.14583333334</v>
+      </c>
+      <c r="B3596" s="2" t="n">
+        <v>46044.1875</v>
+      </c>
+      <c r="C3596" t="n">
+        <v>85.06</v>
+      </c>
+    </row>
+    <row r="3597">
+      <c r="A3597" s="2" t="n">
+        <v>46044.15625</v>
+      </c>
+      <c r="B3597" s="2" t="n">
+        <v>46044.19791666666</v>
+      </c>
+      <c r="C3597" t="n">
+        <v>85.95999999999999</v>
+      </c>
+    </row>
+    <row r="3598">
+      <c r="A3598" s="2" t="n">
+        <v>46044.16666666666</v>
+      </c>
+      <c r="B3598" s="2" t="n">
+        <v>46044.20833333334</v>
+      </c>
+      <c r="C3598" t="n">
+        <v>84.86</v>
+      </c>
+    </row>
+    <row r="3599">
+      <c r="A3599" s="2" t="n">
+        <v>46044.17708333334</v>
+      </c>
+      <c r="B3599" s="2" t="n">
+        <v>46044.21875</v>
+      </c>
+      <c r="C3599" t="n">
+        <v>82.98</v>
+      </c>
+    </row>
+    <row r="3600">
+      <c r="A3600" s="2" t="n">
+        <v>46044.1875</v>
+      </c>
+      <c r="B3600" s="2" t="n">
+        <v>46044.22916666666</v>
+      </c>
+      <c r="C3600" t="n">
+        <v>84.89</v>
+      </c>
+    </row>
+    <row r="3601">
+      <c r="A3601" s="2" t="n">
+        <v>46044.19791666666</v>
+      </c>
+      <c r="B3601" s="2" t="n">
+        <v>46044.23958333334</v>
+      </c>
+      <c r="C3601" t="n">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="3602">
+      <c r="A3602" s="2" t="n">
+        <v>46044.20833333334</v>
+      </c>
+      <c r="B3602" s="2" t="n">
+        <v>46044.25</v>
+      </c>
+      <c r="C3602" t="n">
+        <v>85.23</v>
+      </c>
+    </row>
+    <row r="3603">
+      <c r="A3603" s="2" t="n">
+        <v>46044.21875</v>
+      </c>
+      <c r="B3603" s="2" t="n">
+        <v>46044.26041666666</v>
+      </c>
+      <c r="C3603" t="n">
+        <v>88.73</v>
+      </c>
+    </row>
+    <row r="3604">
+      <c r="A3604" s="2" t="n">
+        <v>46044.22916666666</v>
+      </c>
+      <c r="B3604" s="2" t="n">
+        <v>46044.27083333334</v>
+      </c>
+      <c r="C3604" t="n">
+        <v>101.37</v>
+      </c>
+    </row>
+    <row r="3605">
+      <c r="A3605" s="2" t="n">
+        <v>46044.23958333334</v>
+      </c>
+      <c r="B3605" s="2" t="n">
+        <v>46044.28125</v>
+      </c>
+      <c r="C3605" t="n">
+        <v>111.26</v>
+      </c>
+    </row>
+    <row r="3606">
+      <c r="A3606" s="2" t="n">
+        <v>46044.25</v>
+      </c>
+      <c r="B3606" s="2" t="n">
+        <v>46044.29166666666</v>
+      </c>
+      <c r="C3606" t="n">
+        <v>97.34999999999999</v>
+      </c>
+    </row>
+    <row r="3607">
+      <c r="A3607" s="2" t="n">
+        <v>46044.26041666666</v>
+      </c>
+      <c r="B3607" s="2" t="n">
+        <v>46044.30208333334</v>
+      </c>
+      <c r="C3607" t="n">
+        <v>104.82</v>
+      </c>
+    </row>
+    <row r="3608">
+      <c r="A3608" s="2" t="n">
+        <v>46044.27083333334</v>
+      </c>
+      <c r="B3608" s="2" t="n">
+        <v>46044.3125</v>
+      </c>
+      <c r="C3608" t="n">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="3609">
+      <c r="A3609" s="2" t="n">
+        <v>46044.28125</v>
+      </c>
+      <c r="B3609" s="2" t="n">
+        <v>46044.32291666666</v>
+      </c>
+      <c r="C3609" t="n">
+        <v>119.13</v>
+      </c>
+    </row>
+    <row r="3610">
+      <c r="A3610" s="2" t="n">
+        <v>46044.29166666666</v>
+      </c>
+      <c r="B3610" s="2" t="n">
+        <v>46044.33333333334</v>
+      </c>
+      <c r="C3610" t="n">
+        <v>135.01</v>
+      </c>
+    </row>
+    <row r="3611">
+      <c r="A3611" s="2" t="n">
+        <v>46044.30208333334</v>
+      </c>
+      <c r="B3611" s="2" t="n">
+        <v>46044.34375</v>
+      </c>
+      <c r="C3611" t="n">
+        <v>143.18</v>
+      </c>
+    </row>
+    <row r="3612">
+      <c r="A3612" s="2" t="n">
+        <v>46044.3125</v>
+      </c>
+      <c r="B3612" s="2" t="n">
+        <v>46044.35416666666</v>
+      </c>
+      <c r="C3612" t="n">
+        <v>128.97</v>
+      </c>
+    </row>
+    <row r="3613">
+      <c r="A3613" s="2" t="n">
+        <v>46044.32291666666</v>
+      </c>
+      <c r="B3613" s="2" t="n">
+        <v>46044.36458333334</v>
+      </c>
+      <c r="C3613" t="n">
+        <v>122.18</v>
+      </c>
+    </row>
+    <row r="3614">
+      <c r="A3614" s="2" t="n">
+        <v>46044.33333333334</v>
+      </c>
+      <c r="B3614" s="2" t="n">
+        <v>46044.375</v>
+      </c>
+      <c r="C3614" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="3615">
+      <c r="A3615" s="2" t="n">
+        <v>46044.34375</v>
+      </c>
+      <c r="B3615" s="2" t="n">
+        <v>46044.38541666666</v>
+      </c>
+      <c r="C3615" t="n">
+        <v>115.67</v>
+      </c>
+    </row>
+    <row r="3616">
+      <c r="A3616" s="2" t="n">
+        <v>46044.35416666666</v>
+      </c>
+      <c r="B3616" s="2" t="n">
+        <v>46044.39583333334</v>
+      </c>
+      <c r="C3616" t="n">
+        <v>112.61</v>
+      </c>
+    </row>
+    <row r="3617">
+      <c r="A3617" s="2" t="n">
+        <v>46044.36458333334</v>
+      </c>
+      <c r="B3617" s="2" t="n">
+        <v>46044.40625</v>
+      </c>
+      <c r="C3617" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3618">
+      <c r="A3618" s="2" t="n">
+        <v>46044.375</v>
+      </c>
+      <c r="B3618" s="2" t="n">
+        <v>46044.41666666666</v>
+      </c>
+      <c r="C3618" t="n">
+        <v>109.02</v>
+      </c>
+    </row>
+    <row r="3619">
+      <c r="A3619" s="2" t="n">
+        <v>46044.38541666666</v>
+      </c>
+      <c r="B3619" s="2" t="n">
+        <v>46044.42708333334</v>
+      </c>
+      <c r="C3619" t="n">
+        <v>98.59</v>
+      </c>
+    </row>
+    <row r="3620">
+      <c r="A3620" s="2" t="n">
+        <v>46044.39583333334</v>
+      </c>
+      <c r="B3620" s="2" t="n">
+        <v>46044.4375</v>
+      </c>
+      <c r="C3620" t="n">
+        <v>98.33</v>
+      </c>
+    </row>
+    <row r="3621">
+      <c r="A3621" s="2" t="n">
+        <v>46044.40625</v>
+      </c>
+      <c r="B3621" s="2" t="n">
+        <v>46044.44791666666</v>
+      </c>
+      <c r="C3621" t="n">
+        <v>94.34</v>
+      </c>
+    </row>
+    <row r="3622">
+      <c r="A3622" s="2" t="n">
+        <v>46044.41666666666</v>
+      </c>
+      <c r="B3622" s="2" t="n">
+        <v>46044.45833333334</v>
+      </c>
+      <c r="C3622" t="n">
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="3623">
+      <c r="A3623" s="2" t="n">
+        <v>46044.42708333334</v>
+      </c>
+      <c r="B3623" s="2" t="n">
+        <v>46044.46875</v>
+      </c>
+      <c r="C3623" t="n">
+        <v>89.73999999999999</v>
+      </c>
+    </row>
+    <row r="3624">
+      <c r="A3624" s="2" t="n">
+        <v>46044.4375</v>
+      </c>
+      <c r="B3624" s="2" t="n">
+        <v>46044.47916666666</v>
+      </c>
+      <c r="C3624" t="n">
+        <v>89.94</v>
+      </c>
+    </row>
+    <row r="3625">
+      <c r="A3625" s="2" t="n">
+        <v>46044.44791666666</v>
+      </c>
+      <c r="B3625" s="2" t="n">
+        <v>46044.48958333334</v>
+      </c>
+      <c r="C3625" t="n">
+        <v>87.45</v>
+      </c>
+    </row>
+    <row r="3626">
+      <c r="A3626" s="2" t="n">
+        <v>46044.45833333334</v>
+      </c>
+      <c r="B3626" s="2" t="n">
+        <v>46044.5</v>
+      </c>
+      <c r="C3626" t="n">
+        <v>90.73</v>
+      </c>
+    </row>
+    <row r="3627">
+      <c r="A3627" s="2" t="n">
+        <v>46044.46875</v>
+      </c>
+      <c r="B3627" s="2" t="n">
+        <v>46044.51041666666</v>
+      </c>
+      <c r="C3627" t="n">
+        <v>87.01000000000001</v>
+      </c>
+    </row>
+    <row r="3628">
+      <c r="A3628" s="2" t="n">
+        <v>46044.47916666666</v>
+      </c>
+      <c r="B3628" s="2" t="n">
+        <v>46044.52083333334</v>
+      </c>
+      <c r="C3628" t="n">
+        <v>86.53</v>
+      </c>
+    </row>
+    <row r="3629">
+      <c r="A3629" s="2" t="n">
+        <v>46044.48958333334</v>
+      </c>
+      <c r="B3629" s="2" t="n">
+        <v>46044.53125</v>
+      </c>
+      <c r="C3629" t="n">
+        <v>85.88</v>
+      </c>
+    </row>
+    <row r="3630">
+      <c r="A3630" s="2" t="n">
+        <v>46044.5</v>
+      </c>
+      <c r="B3630" s="2" t="n">
+        <v>46044.54166666666</v>
+      </c>
+      <c r="C3630" t="n">
+        <v>89.94</v>
+      </c>
+    </row>
+    <row r="3631">
+      <c r="A3631" s="2" t="n">
+        <v>46044.51041666666</v>
+      </c>
+      <c r="B3631" s="2" t="n">
+        <v>46044.55208333334</v>
+      </c>
+      <c r="C3631" t="n">
+        <v>90.76000000000001</v>
+      </c>
+    </row>
+    <row r="3632">
+      <c r="A3632" s="2" t="n">
+        <v>46044.52083333334</v>
+      </c>
+      <c r="B3632" s="2" t="n">
+        <v>46044.5625</v>
+      </c>
+      <c r="C3632" t="n">
+        <v>90.06</v>
+      </c>
+    </row>
+    <row r="3633">
+      <c r="A3633" s="2" t="n">
+        <v>46044.53125</v>
+      </c>
+      <c r="B3633" s="2" t="n">
+        <v>46044.57291666666</v>
+      </c>
+      <c r="C3633" t="n">
+        <v>90.17</v>
+      </c>
+    </row>
+    <row r="3634">
+      <c r="A3634" s="2" t="n">
+        <v>46044.54166666666</v>
+      </c>
+      <c r="B3634" s="2" t="n">
+        <v>46044.58333333334</v>
+      </c>
+      <c r="C3634" t="n">
+        <v>90.67</v>
+      </c>
+    </row>
+    <row r="3635">
+      <c r="A3635" s="2" t="n">
+        <v>46044.55208333334</v>
+      </c>
+      <c r="B3635" s="2" t="n">
+        <v>46044.59375</v>
+      </c>
+      <c r="C3635" t="n">
+        <v>97.09</v>
+      </c>
+    </row>
+    <row r="3636">
+      <c r="A3636" s="2" t="n">
+        <v>46044.5625</v>
+      </c>
+      <c r="B3636" s="2" t="n">
+        <v>46044.60416666666</v>
+      </c>
+      <c r="C3636" t="n">
+        <v>96.87</v>
+      </c>
+    </row>
+    <row r="3637">
+      <c r="A3637" s="2" t="n">
+        <v>46044.57291666666</v>
+      </c>
+      <c r="B3637" s="2" t="n">
+        <v>46044.61458333334</v>
+      </c>
+      <c r="C3637" t="n">
+        <v>101.49</v>
+      </c>
+    </row>
+    <row r="3638">
+      <c r="A3638" s="2" t="n">
+        <v>46044.58333333334</v>
+      </c>
+      <c r="B3638" s="2" t="n">
+        <v>46044.625</v>
+      </c>
+      <c r="C3638" t="n">
+        <v>95.83</v>
+      </c>
+    </row>
+    <row r="3639">
+      <c r="A3639" s="2" t="n">
+        <v>46044.59375</v>
+      </c>
+      <c r="B3639" s="2" t="n">
+        <v>46044.63541666666</v>
+      </c>
+      <c r="C3639" t="n">
+        <v>101.88</v>
+      </c>
+    </row>
+    <row r="3640">
+      <c r="A3640" s="2" t="n">
+        <v>46044.60416666666</v>
+      </c>
+      <c r="B3640" s="2" t="n">
+        <v>46044.64583333334</v>
+      </c>
+      <c r="C3640" t="n">
+        <v>108.25</v>
+      </c>
+    </row>
+    <row r="3641">
+      <c r="A3641" s="2" t="n">
+        <v>46044.61458333334</v>
+      </c>
+      <c r="B3641" s="2" t="n">
+        <v>46044.65625</v>
+      </c>
+      <c r="C3641" t="n">
+        <v>113.86</v>
+      </c>
+    </row>
+    <row r="3642">
+      <c r="A3642" s="2" t="n">
+        <v>46044.625</v>
+      </c>
+      <c r="B3642" s="2" t="n">
+        <v>46044.66666666666</v>
+      </c>
+      <c r="C3642" t="n">
+        <v>110.07</v>
+      </c>
+    </row>
+    <row r="3643">
+      <c r="A3643" s="2" t="n">
+        <v>46044.63541666666</v>
+      </c>
+      <c r="B3643" s="2" t="n">
+        <v>46044.67708333334</v>
+      </c>
+      <c r="C3643" t="n">
+        <v>123.16</v>
+      </c>
+    </row>
+    <row r="3644">
+      <c r="A3644" s="2" t="n">
+        <v>46044.64583333334</v>
+      </c>
+      <c r="B3644" s="2" t="n">
+        <v>46044.6875</v>
+      </c>
+      <c r="C3644" t="n">
+        <v>136.94</v>
+      </c>
+    </row>
+    <row r="3645">
+      <c r="A3645" s="2" t="n">
+        <v>46044.65625</v>
+      </c>
+      <c r="B3645" s="2" t="n">
+        <v>46044.69791666666</v>
+      </c>
+      <c r="C3645" t="n">
+        <v>127.61</v>
+      </c>
+    </row>
+    <row r="3646">
+      <c r="A3646" s="2" t="n">
+        <v>46044.66666666666</v>
+      </c>
+      <c r="B3646" s="2" t="n">
+        <v>46044.70833333334</v>
+      </c>
+      <c r="C3646" t="n">
+        <v>123.63</v>
+      </c>
+    </row>
+    <row r="3647">
+      <c r="A3647" s="2" t="n">
+        <v>46044.67708333334</v>
+      </c>
+      <c r="B3647" s="2" t="n">
+        <v>46044.71875</v>
+      </c>
+      <c r="C3647" t="n">
+        <v>131.92</v>
+      </c>
+    </row>
+    <row r="3648">
+      <c r="A3648" s="2" t="n">
+        <v>46044.6875</v>
+      </c>
+      <c r="B3648" s="2" t="n">
+        <v>46044.72916666666</v>
+      </c>
+      <c r="C3648" t="n">
+        <v>136.64</v>
+      </c>
+    </row>
+    <row r="3649">
+      <c r="A3649" s="2" t="n">
+        <v>46044.69791666666</v>
+      </c>
+      <c r="B3649" s="2" t="n">
+        <v>46044.73958333334</v>
+      </c>
+      <c r="C3649" t="n">
+        <v>134.98</v>
+      </c>
+    </row>
+    <row r="3650">
+      <c r="A3650" s="2" t="n">
+        <v>46044.70833333334</v>
+      </c>
+      <c r="B3650" s="2" t="n">
+        <v>46044.75</v>
+      </c>
+      <c r="C3650" t="n">
+        <v>126.39</v>
+      </c>
+    </row>
+    <row r="3651">
+      <c r="A3651" s="2" t="n">
+        <v>46044.71875</v>
+      </c>
+      <c r="B3651" s="2" t="n">
+        <v>46044.76041666666</v>
+      </c>
+      <c r="C3651" t="n">
+        <v>127.39</v>
+      </c>
+    </row>
+    <row r="3652">
+      <c r="A3652" s="2" t="n">
+        <v>46044.72916666666</v>
+      </c>
+      <c r="B3652" s="2" t="n">
+        <v>46044.77083333334</v>
+      </c>
+      <c r="C3652" t="n">
+        <v>127.42</v>
+      </c>
+    </row>
+    <row r="3653">
+      <c r="A3653" s="2" t="n">
+        <v>46044.73958333334</v>
+      </c>
+      <c r="B3653" s="2" t="n">
+        <v>46044.78125</v>
+      </c>
+      <c r="C3653" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3654">
+      <c r="A3654" s="2" t="n">
+        <v>46044.75</v>
+      </c>
+      <c r="B3654" s="2" t="n">
+        <v>46044.79166666666</v>
+      </c>
+      <c r="C3654" t="n">
+        <v>128.65</v>
+      </c>
+    </row>
+    <row r="3655">
+      <c r="A3655" s="2" t="n">
+        <v>46044.76041666666</v>
+      </c>
+      <c r="B3655" s="2" t="n">
+        <v>46044.80208333334</v>
+      </c>
+      <c r="C3655" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3656">
+      <c r="A3656" s="2" t="n">
+        <v>46044.77083333334</v>
+      </c>
+      <c r="B3656" s="2" t="n">
+        <v>46044.8125</v>
+      </c>
+      <c r="C3656" t="n">
+        <v>122.67</v>
+      </c>
+    </row>
+    <row r="3657">
+      <c r="A3657" s="2" t="n">
+        <v>46044.78125</v>
+      </c>
+      <c r="B3657" s="2" t="n">
+        <v>46044.82291666666</v>
+      </c>
+      <c r="C3657" t="n">
+        <v>112.81</v>
+      </c>
+    </row>
+    <row r="3658">
+      <c r="A3658" s="2" t="n">
+        <v>46044.79166666666</v>
+      </c>
+      <c r="B3658" s="2" t="n">
+        <v>46044.83333333334</v>
+      </c>
+      <c r="C3658" t="n">
+        <v>115.91</v>
+      </c>
+    </row>
+    <row r="3659">
+      <c r="A3659" s="2" t="n">
+        <v>46044.80208333334</v>
+      </c>
+      <c r="B3659" s="2" t="n">
+        <v>46044.84375</v>
+      </c>
+      <c r="C3659" t="n">
+        <v>108.31</v>
+      </c>
+    </row>
+    <row r="3660">
+      <c r="A3660" s="2" t="n">
+        <v>46044.8125</v>
+      </c>
+      <c r="B3660" s="2" t="n">
+        <v>46044.85416666666</v>
+      </c>
+      <c r="C3660" t="n">
+        <v>108.1</v>
+      </c>
+    </row>
+    <row r="3661">
+      <c r="A3661" s="2" t="n">
+        <v>46044.82291666666</v>
+      </c>
+      <c r="B3661" s="2" t="n">
+        <v>46044.86458333334</v>
+      </c>
+      <c r="C3661" t="n">
+        <v>106.14</v>
+      </c>
+    </row>
+    <row r="3662">
+      <c r="A3662" s="2" t="n">
+        <v>46044.83333333334</v>
+      </c>
+      <c r="B3662" s="2" t="n">
+        <v>46044.875</v>
+      </c>
+      <c r="C3662" t="n">
+        <v>120.33</v>
+      </c>
+    </row>
+    <row r="3663">
+      <c r="A3663" s="2" t="n">
+        <v>46044.84375</v>
+      </c>
+      <c r="B3663" s="2" t="n">
+        <v>46044.88541666666</v>
+      </c>
+      <c r="C3663" t="n">
+        <v>108.04</v>
+      </c>
+    </row>
+    <row r="3664">
+      <c r="A3664" s="2" t="n">
+        <v>46044.85416666666</v>
+      </c>
+      <c r="B3664" s="2" t="n">
+        <v>46044.89583333334</v>
+      </c>
+      <c r="C3664" t="n">
+        <v>101.84</v>
+      </c>
+    </row>
+    <row r="3665">
+      <c r="A3665" s="2" t="n">
+        <v>46044.86458333334</v>
+      </c>
+      <c r="B3665" s="2" t="n">
+        <v>46044.90625</v>
+      </c>
+      <c r="C3665" t="n">
+        <v>97.44</v>
+      </c>
+    </row>
+    <row r="3666">
+      <c r="A3666" s="2" t="n">
+        <v>46044.875</v>
+      </c>
+      <c r="B3666" s="2" t="n">
+        <v>46044.91666666666</v>
+      </c>
+      <c r="C3666" t="n">
+        <v>102.68</v>
+      </c>
+    </row>
+    <row r="3667">
+      <c r="A3667" s="2" t="n">
+        <v>46044.88541666666</v>
+      </c>
+      <c r="B3667" s="2" t="n">
+        <v>46044.92708333334</v>
+      </c>
+      <c r="C3667" t="n">
+        <v>101.91</v>
+      </c>
+    </row>
+    <row r="3668">
+      <c r="A3668" s="2" t="n">
+        <v>46044.89583333334</v>
+      </c>
+      <c r="B3668" s="2" t="n">
+        <v>46044.9375</v>
+      </c>
+      <c r="C3668" t="n">
+        <v>108.95</v>
+      </c>
+    </row>
+    <row r="3669">
+      <c r="A3669" s="2" t="n">
+        <v>46044.90625</v>
+      </c>
+      <c r="B3669" s="2" t="n">
+        <v>46044.94791666666</v>
+      </c>
+      <c r="C3669" t="n">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="3670">
+      <c r="A3670" s="2" t="n">
+        <v>46044.91666666666</v>
+      </c>
+      <c r="B3670" s="2" t="n">
+        <v>46044.95833333334</v>
+      </c>
+      <c r="C3670" t="n">
+        <v>102.67</v>
+      </c>
+    </row>
+    <row r="3671">
+      <c r="A3671" s="2" t="n">
+        <v>46044.92708333334</v>
+      </c>
+      <c r="B3671" s="2" t="n">
+        <v>46044.96875</v>
+      </c>
+      <c r="C3671" t="n">
+        <v>96.56</v>
+      </c>
+    </row>
+    <row r="3672">
+      <c r="A3672" s="2" t="n">
+        <v>46044.9375</v>
+      </c>
+      <c r="B3672" s="2" t="n">
+        <v>46044.97916666666</v>
+      </c>
+      <c r="C3672" t="n">
+        <v>99.45</v>
+      </c>
+    </row>
+    <row r="3673">
+      <c r="A3673" s="2" t="n">
+        <v>46044.94791666666</v>
+      </c>
+      <c r="B3673" s="2" t="n">
+        <v>46044.98958333334</v>
+      </c>
+      <c r="C3673" t="n">
+        <v>90.45999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update XLSX via API 28-01-2026, 08:49:31
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Update XLSX via API 30-01-2026, 09:15:44
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Update XLSX via API 09-02-2026, 12:53:11
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Update XLSX via API 09-02-2026, 14:06:12
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3840"/>
+  <dimension ref="A1:C3744"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41577,1062 +41577,6 @@
         <v>90.45999999999999</v>
       </c>
     </row>
-    <row r="3745">
-      <c r="A3745" s="2" t="n">
-        <v>46060.95833333334</v>
-      </c>
-      <c r="B3745" s="2" t="n">
-        <v>46061</v>
-      </c>
-      <c r="C3745" t="n">
-        <v>108.87</v>
-      </c>
-    </row>
-    <row r="3746">
-      <c r="A3746" s="2" t="n">
-        <v>46060.96875</v>
-      </c>
-      <c r="B3746" s="2" t="n">
-        <v>46061.01041666666</v>
-      </c>
-      <c r="C3746" t="n">
-        <v>101.13</v>
-      </c>
-    </row>
-    <row r="3747">
-      <c r="A3747" s="2" t="n">
-        <v>46060.97916666666</v>
-      </c>
-      <c r="B3747" s="2" t="n">
-        <v>46061.02083333334</v>
-      </c>
-      <c r="C3747" t="n">
-        <v>97.81999999999999</v>
-      </c>
-    </row>
-    <row r="3748">
-      <c r="A3748" s="2" t="n">
-        <v>46060.98958333334</v>
-      </c>
-      <c r="B3748" s="2" t="n">
-        <v>46061.03125</v>
-      </c>
-      <c r="C3748" t="n">
-        <v>93.06999999999999</v>
-      </c>
-    </row>
-    <row r="3749">
-      <c r="A3749" s="2" t="n">
-        <v>46061</v>
-      </c>
-      <c r="B3749" s="2" t="n">
-        <v>46061.04166666666</v>
-      </c>
-      <c r="C3749" t="n">
-        <v>97.79000000000001</v>
-      </c>
-    </row>
-    <row r="3750">
-      <c r="A3750" s="2" t="n">
-        <v>46061.01041666666</v>
-      </c>
-      <c r="B3750" s="2" t="n">
-        <v>46061.05208333334</v>
-      </c>
-      <c r="C3750" t="n">
-        <v>98.66</v>
-      </c>
-    </row>
-    <row r="3751">
-      <c r="A3751" s="2" t="n">
-        <v>46061.02083333334</v>
-      </c>
-      <c r="B3751" s="2" t="n">
-        <v>46061.0625</v>
-      </c>
-      <c r="C3751" t="n">
-        <v>97.09999999999999</v>
-      </c>
-    </row>
-    <row r="3752">
-      <c r="A3752" s="2" t="n">
-        <v>46061.03125</v>
-      </c>
-      <c r="B3752" s="2" t="n">
-        <v>46061.07291666666</v>
-      </c>
-      <c r="C3752" t="n">
-        <v>95.20999999999999</v>
-      </c>
-    </row>
-    <row r="3753">
-      <c r="A3753" s="2" t="n">
-        <v>46061.04166666666</v>
-      </c>
-      <c r="B3753" s="2" t="n">
-        <v>46061.08333333334</v>
-      </c>
-      <c r="C3753" t="n">
-        <v>98.05</v>
-      </c>
-    </row>
-    <row r="3754">
-      <c r="A3754" s="2" t="n">
-        <v>46061.05208333334</v>
-      </c>
-      <c r="B3754" s="2" t="n">
-        <v>46061.09375</v>
-      </c>
-      <c r="C3754" t="n">
-        <v>95.23</v>
-      </c>
-    </row>
-    <row r="3755">
-      <c r="A3755" s="2" t="n">
-        <v>46061.0625</v>
-      </c>
-      <c r="B3755" s="2" t="n">
-        <v>46061.10416666666</v>
-      </c>
-      <c r="C3755" t="n">
-        <v>92.69</v>
-      </c>
-    </row>
-    <row r="3756">
-      <c r="A3756" s="2" t="n">
-        <v>46061.07291666666</v>
-      </c>
-      <c r="B3756" s="2" t="n">
-        <v>46061.11458333334</v>
-      </c>
-      <c r="C3756" t="n">
-        <v>91.63</v>
-      </c>
-    </row>
-    <row r="3757">
-      <c r="A3757" s="2" t="n">
-        <v>46061.08333333334</v>
-      </c>
-      <c r="B3757" s="2" t="n">
-        <v>46061.125</v>
-      </c>
-      <c r="C3757" t="n">
-        <v>93.48999999999999</v>
-      </c>
-    </row>
-    <row r="3758">
-      <c r="A3758" s="2" t="n">
-        <v>46061.09375</v>
-      </c>
-      <c r="B3758" s="2" t="n">
-        <v>46061.13541666666</v>
-      </c>
-      <c r="C3758" t="n">
-        <v>92.25</v>
-      </c>
-    </row>
-    <row r="3759">
-      <c r="A3759" s="2" t="n">
-        <v>46061.10416666666</v>
-      </c>
-      <c r="B3759" s="2" t="n">
-        <v>46061.14583333334</v>
-      </c>
-      <c r="C3759" t="n">
-        <v>91.13</v>
-      </c>
-    </row>
-    <row r="3760">
-      <c r="A3760" s="2" t="n">
-        <v>46061.11458333334</v>
-      </c>
-      <c r="B3760" s="2" t="n">
-        <v>46061.15625</v>
-      </c>
-      <c r="C3760" t="n">
-        <v>91.61</v>
-      </c>
-    </row>
-    <row r="3761">
-      <c r="A3761" s="2" t="n">
-        <v>46061.125</v>
-      </c>
-      <c r="B3761" s="2" t="n">
-        <v>46061.16666666666</v>
-      </c>
-      <c r="C3761" t="n">
-        <v>90.34999999999999</v>
-      </c>
-    </row>
-    <row r="3762">
-      <c r="A3762" s="2" t="n">
-        <v>46061.13541666666</v>
-      </c>
-      <c r="B3762" s="2" t="n">
-        <v>46061.17708333334</v>
-      </c>
-      <c r="C3762" t="n">
-        <v>90.43000000000001</v>
-      </c>
-    </row>
-    <row r="3763">
-      <c r="A3763" s="2" t="n">
-        <v>46061.14583333334</v>
-      </c>
-      <c r="B3763" s="2" t="n">
-        <v>46061.1875</v>
-      </c>
-      <c r="C3763" t="n">
-        <v>90.73</v>
-      </c>
-    </row>
-    <row r="3764">
-      <c r="A3764" s="2" t="n">
-        <v>46061.15625</v>
-      </c>
-      <c r="B3764" s="2" t="n">
-        <v>46061.19791666666</v>
-      </c>
-      <c r="C3764" t="n">
-        <v>90.33</v>
-      </c>
-    </row>
-    <row r="3765">
-      <c r="A3765" s="2" t="n">
-        <v>46061.16666666666</v>
-      </c>
-      <c r="B3765" s="2" t="n">
-        <v>46061.20833333334</v>
-      </c>
-      <c r="C3765" t="n">
-        <v>92.12</v>
-      </c>
-    </row>
-    <row r="3766">
-      <c r="A3766" s="2" t="n">
-        <v>46061.17708333334</v>
-      </c>
-      <c r="B3766" s="2" t="n">
-        <v>46061.21875</v>
-      </c>
-      <c r="C3766" t="n">
-        <v>91.44</v>
-      </c>
-    </row>
-    <row r="3767">
-      <c r="A3767" s="2" t="n">
-        <v>46061.1875</v>
-      </c>
-      <c r="B3767" s="2" t="n">
-        <v>46061.22916666666</v>
-      </c>
-      <c r="C3767" t="n">
-        <v>90.36</v>
-      </c>
-    </row>
-    <row r="3768">
-      <c r="A3768" s="2" t="n">
-        <v>46061.19791666666</v>
-      </c>
-      <c r="B3768" s="2" t="n">
-        <v>46061.23958333334</v>
-      </c>
-      <c r="C3768" t="n">
-        <v>91.61</v>
-      </c>
-    </row>
-    <row r="3769">
-      <c r="A3769" s="2" t="n">
-        <v>46061.20833333334</v>
-      </c>
-      <c r="B3769" s="2" t="n">
-        <v>46061.25</v>
-      </c>
-      <c r="C3769" t="n">
-        <v>84.8</v>
-      </c>
-    </row>
-    <row r="3770">
-      <c r="A3770" s="2" t="n">
-        <v>46061.21875</v>
-      </c>
-      <c r="B3770" s="2" t="n">
-        <v>46061.26041666666</v>
-      </c>
-      <c r="C3770" t="n">
-        <v>87.67</v>
-      </c>
-    </row>
-    <row r="3771">
-      <c r="A3771" s="2" t="n">
-        <v>46061.22916666666</v>
-      </c>
-      <c r="B3771" s="2" t="n">
-        <v>46061.27083333334</v>
-      </c>
-      <c r="C3771" t="n">
-        <v>90.98</v>
-      </c>
-    </row>
-    <row r="3772">
-      <c r="A3772" s="2" t="n">
-        <v>46061.23958333334</v>
-      </c>
-      <c r="B3772" s="2" t="n">
-        <v>46061.28125</v>
-      </c>
-      <c r="C3772" t="n">
-        <v>95.95999999999999</v>
-      </c>
-    </row>
-    <row r="3773">
-      <c r="A3773" s="2" t="n">
-        <v>46061.25</v>
-      </c>
-      <c r="B3773" s="2" t="n">
-        <v>46061.29166666666</v>
-      </c>
-      <c r="C3773" t="n">
-        <v>88.2</v>
-      </c>
-    </row>
-    <row r="3774">
-      <c r="A3774" s="2" t="n">
-        <v>46061.26041666666</v>
-      </c>
-      <c r="B3774" s="2" t="n">
-        <v>46061.30208333334</v>
-      </c>
-      <c r="C3774" t="n">
-        <v>91.33</v>
-      </c>
-    </row>
-    <row r="3775">
-      <c r="A3775" s="2" t="n">
-        <v>46061.27083333334</v>
-      </c>
-      <c r="B3775" s="2" t="n">
-        <v>46061.3125</v>
-      </c>
-      <c r="C3775" t="n">
-        <v>94.69</v>
-      </c>
-    </row>
-    <row r="3776">
-      <c r="A3776" s="2" t="n">
-        <v>46061.28125</v>
-      </c>
-      <c r="B3776" s="2" t="n">
-        <v>46061.32291666666</v>
-      </c>
-      <c r="C3776" t="n">
-        <v>99.09999999999999</v>
-      </c>
-    </row>
-    <row r="3777">
-      <c r="A3777" s="2" t="n">
-        <v>46061.29166666666</v>
-      </c>
-      <c r="B3777" s="2" t="n">
-        <v>46061.33333333334</v>
-      </c>
-      <c r="C3777" t="n">
-        <v>94.41</v>
-      </c>
-    </row>
-    <row r="3778">
-      <c r="A3778" s="2" t="n">
-        <v>46061.30208333334</v>
-      </c>
-      <c r="B3778" s="2" t="n">
-        <v>46061.34375</v>
-      </c>
-      <c r="C3778" t="n">
-        <v>98.72</v>
-      </c>
-    </row>
-    <row r="3779">
-      <c r="A3779" s="2" t="n">
-        <v>46061.3125</v>
-      </c>
-      <c r="B3779" s="2" t="n">
-        <v>46061.35416666666</v>
-      </c>
-      <c r="C3779" t="n">
-        <v>100.1</v>
-      </c>
-    </row>
-    <row r="3780">
-      <c r="A3780" s="2" t="n">
-        <v>46061.32291666666</v>
-      </c>
-      <c r="B3780" s="2" t="n">
-        <v>46061.36458333334</v>
-      </c>
-      <c r="C3780" t="n">
-        <v>100.04</v>
-      </c>
-    </row>
-    <row r="3781">
-      <c r="A3781" s="2" t="n">
-        <v>46061.33333333334</v>
-      </c>
-      <c r="B3781" s="2" t="n">
-        <v>46061.375</v>
-      </c>
-      <c r="C3781" t="n">
-        <v>100.16</v>
-      </c>
-    </row>
-    <row r="3782">
-      <c r="A3782" s="2" t="n">
-        <v>46061.34375</v>
-      </c>
-      <c r="B3782" s="2" t="n">
-        <v>46061.38541666666</v>
-      </c>
-      <c r="C3782" t="n">
-        <v>99.87</v>
-      </c>
-    </row>
-    <row r="3783">
-      <c r="A3783" s="2" t="n">
-        <v>46061.35416666666</v>
-      </c>
-      <c r="B3783" s="2" t="n">
-        <v>46061.39583333334</v>
-      </c>
-      <c r="C3783" t="n">
-        <v>99.48999999999999</v>
-      </c>
-    </row>
-    <row r="3784">
-      <c r="A3784" s="2" t="n">
-        <v>46061.36458333334</v>
-      </c>
-      <c r="B3784" s="2" t="n">
-        <v>46061.40625</v>
-      </c>
-      <c r="C3784" t="n">
-        <v>93.78</v>
-      </c>
-    </row>
-    <row r="3785">
-      <c r="A3785" s="2" t="n">
-        <v>46061.375</v>
-      </c>
-      <c r="B3785" s="2" t="n">
-        <v>46061.41666666666</v>
-      </c>
-      <c r="C3785" t="n">
-        <v>100.9</v>
-      </c>
-    </row>
-    <row r="3786">
-      <c r="A3786" s="2" t="n">
-        <v>46061.38541666666</v>
-      </c>
-      <c r="B3786" s="2" t="n">
-        <v>46061.42708333334</v>
-      </c>
-      <c r="C3786" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3787">
-      <c r="A3787" s="2" t="n">
-        <v>46061.39583333334</v>
-      </c>
-      <c r="B3787" s="2" t="n">
-        <v>46061.4375</v>
-      </c>
-      <c r="C3787" t="n">
-        <v>94.86</v>
-      </c>
-    </row>
-    <row r="3788">
-      <c r="A3788" s="2" t="n">
-        <v>46061.40625</v>
-      </c>
-      <c r="B3788" s="2" t="n">
-        <v>46061.44791666666</v>
-      </c>
-      <c r="C3788" t="n">
-        <v>93.12</v>
-      </c>
-    </row>
-    <row r="3789">
-      <c r="A3789" s="2" t="n">
-        <v>46061.41666666666</v>
-      </c>
-      <c r="B3789" s="2" t="n">
-        <v>46061.45833333334</v>
-      </c>
-      <c r="C3789" t="n">
-        <v>96.90000000000001</v>
-      </c>
-    </row>
-    <row r="3790">
-      <c r="A3790" s="2" t="n">
-        <v>46061.42708333334</v>
-      </c>
-      <c r="B3790" s="2" t="n">
-        <v>46061.46875</v>
-      </c>
-      <c r="C3790" t="n">
-        <v>93.98</v>
-      </c>
-    </row>
-    <row r="3791">
-      <c r="A3791" s="2" t="n">
-        <v>46061.4375</v>
-      </c>
-      <c r="B3791" s="2" t="n">
-        <v>46061.47916666666</v>
-      </c>
-      <c r="C3791" t="n">
-        <v>92.53</v>
-      </c>
-    </row>
-    <row r="3792">
-      <c r="A3792" s="2" t="n">
-        <v>46061.44791666666</v>
-      </c>
-      <c r="B3792" s="2" t="n">
-        <v>46061.48958333334</v>
-      </c>
-      <c r="C3792" t="n">
-        <v>90.44</v>
-      </c>
-    </row>
-    <row r="3793">
-      <c r="A3793" s="2" t="n">
-        <v>46061.45833333334</v>
-      </c>
-      <c r="B3793" s="2" t="n">
-        <v>46061.5</v>
-      </c>
-      <c r="C3793" t="n">
-        <v>92.03</v>
-      </c>
-    </row>
-    <row r="3794">
-      <c r="A3794" s="2" t="n">
-        <v>46061.46875</v>
-      </c>
-      <c r="B3794" s="2" t="n">
-        <v>46061.51041666666</v>
-      </c>
-      <c r="C3794" t="n">
-        <v>90.5</v>
-      </c>
-    </row>
-    <row r="3795">
-      <c r="A3795" s="2" t="n">
-        <v>46061.47916666666</v>
-      </c>
-      <c r="B3795" s="2" t="n">
-        <v>46061.52083333334</v>
-      </c>
-      <c r="C3795" t="n">
-        <v>92.56</v>
-      </c>
-    </row>
-    <row r="3796">
-      <c r="A3796" s="2" t="n">
-        <v>46061.48958333334</v>
-      </c>
-      <c r="B3796" s="2" t="n">
-        <v>46061.53125</v>
-      </c>
-      <c r="C3796" t="n">
-        <v>89.59</v>
-      </c>
-    </row>
-    <row r="3797">
-      <c r="A3797" s="2" t="n">
-        <v>46061.5</v>
-      </c>
-      <c r="B3797" s="2" t="n">
-        <v>46061.54166666666</v>
-      </c>
-      <c r="C3797" t="n">
-        <v>90.8</v>
-      </c>
-    </row>
-    <row r="3798">
-      <c r="A3798" s="2" t="n">
-        <v>46061.51041666666</v>
-      </c>
-      <c r="B3798" s="2" t="n">
-        <v>46061.55208333334</v>
-      </c>
-      <c r="C3798" t="n">
-        <v>88.97</v>
-      </c>
-    </row>
-    <row r="3799">
-      <c r="A3799" s="2" t="n">
-        <v>46061.52083333334</v>
-      </c>
-      <c r="B3799" s="2" t="n">
-        <v>46061.5625</v>
-      </c>
-      <c r="C3799" t="n">
-        <v>90.88</v>
-      </c>
-    </row>
-    <row r="3800">
-      <c r="A3800" s="2" t="n">
-        <v>46061.53125</v>
-      </c>
-      <c r="B3800" s="2" t="n">
-        <v>46061.57291666666</v>
-      </c>
-      <c r="C3800" t="n">
-        <v>89.17</v>
-      </c>
-    </row>
-    <row r="3801">
-      <c r="A3801" s="2" t="n">
-        <v>46061.54166666666</v>
-      </c>
-      <c r="B3801" s="2" t="n">
-        <v>46061.58333333334</v>
-      </c>
-      <c r="C3801" t="n">
-        <v>88.76000000000001</v>
-      </c>
-    </row>
-    <row r="3802">
-      <c r="A3802" s="2" t="n">
-        <v>46061.55208333334</v>
-      </c>
-      <c r="B3802" s="2" t="n">
-        <v>46061.59375</v>
-      </c>
-      <c r="C3802" t="n">
-        <v>89.90000000000001</v>
-      </c>
-    </row>
-    <row r="3803">
-      <c r="A3803" s="2" t="n">
-        <v>46061.5625</v>
-      </c>
-      <c r="B3803" s="2" t="n">
-        <v>46061.60416666666</v>
-      </c>
-      <c r="C3803" t="n">
-        <v>91.29000000000001</v>
-      </c>
-    </row>
-    <row r="3804">
-      <c r="A3804" s="2" t="n">
-        <v>46061.57291666666</v>
-      </c>
-      <c r="B3804" s="2" t="n">
-        <v>46061.61458333334</v>
-      </c>
-      <c r="C3804" t="n">
-        <v>93.73</v>
-      </c>
-    </row>
-    <row r="3805">
-      <c r="A3805" s="2" t="n">
-        <v>46061.58333333334</v>
-      </c>
-      <c r="B3805" s="2" t="n">
-        <v>46061.625</v>
-      </c>
-      <c r="C3805" t="n">
-        <v>92.69</v>
-      </c>
-    </row>
-    <row r="3806">
-      <c r="A3806" s="2" t="n">
-        <v>46061.59375</v>
-      </c>
-      <c r="B3806" s="2" t="n">
-        <v>46061.63541666666</v>
-      </c>
-      <c r="C3806" t="n">
-        <v>96.51000000000001</v>
-      </c>
-    </row>
-    <row r="3807">
-      <c r="A3807" s="2" t="n">
-        <v>46061.60416666666</v>
-      </c>
-      <c r="B3807" s="2" t="n">
-        <v>46061.64583333334</v>
-      </c>
-      <c r="C3807" t="n">
-        <v>99.09999999999999</v>
-      </c>
-    </row>
-    <row r="3808">
-      <c r="A3808" s="2" t="n">
-        <v>46061.61458333334</v>
-      </c>
-      <c r="B3808" s="2" t="n">
-        <v>46061.65625</v>
-      </c>
-      <c r="C3808" t="n">
-        <v>105.63</v>
-      </c>
-    </row>
-    <row r="3809">
-      <c r="A3809" s="2" t="n">
-        <v>46061.625</v>
-      </c>
-      <c r="B3809" s="2" t="n">
-        <v>46061.66666666666</v>
-      </c>
-      <c r="C3809" t="n">
-        <v>92.94</v>
-      </c>
-    </row>
-    <row r="3810">
-      <c r="A3810" s="2" t="n">
-        <v>46061.63541666666</v>
-      </c>
-      <c r="B3810" s="2" t="n">
-        <v>46061.67708333334</v>
-      </c>
-      <c r="C3810" t="n">
-        <v>100.57</v>
-      </c>
-    </row>
-    <row r="3811">
-      <c r="A3811" s="2" t="n">
-        <v>46061.64583333334</v>
-      </c>
-      <c r="B3811" s="2" t="n">
-        <v>46061.6875</v>
-      </c>
-      <c r="C3811" t="n">
-        <v>107.46</v>
-      </c>
-    </row>
-    <row r="3812">
-      <c r="A3812" s="2" t="n">
-        <v>46061.65625</v>
-      </c>
-      <c r="B3812" s="2" t="n">
-        <v>46061.69791666666</v>
-      </c>
-      <c r="C3812" t="n">
-        <v>118.19</v>
-      </c>
-    </row>
-    <row r="3813">
-      <c r="A3813" s="2" t="n">
-        <v>46061.66666666666</v>
-      </c>
-      <c r="B3813" s="2" t="n">
-        <v>46061.70833333334</v>
-      </c>
-      <c r="C3813" t="n">
-        <v>111.91</v>
-      </c>
-    </row>
-    <row r="3814">
-      <c r="A3814" s="2" t="n">
-        <v>46061.67708333334</v>
-      </c>
-      <c r="B3814" s="2" t="n">
-        <v>46061.71875</v>
-      </c>
-      <c r="C3814" t="n">
-        <v>120.09</v>
-      </c>
-    </row>
-    <row r="3815">
-      <c r="A3815" s="2" t="n">
-        <v>46061.6875</v>
-      </c>
-      <c r="B3815" s="2" t="n">
-        <v>46061.72916666666</v>
-      </c>
-      <c r="C3815" t="n">
-        <v>125.41</v>
-      </c>
-    </row>
-    <row r="3816">
-      <c r="A3816" s="2" t="n">
-        <v>46061.69791666666</v>
-      </c>
-      <c r="B3816" s="2" t="n">
-        <v>46061.73958333334</v>
-      </c>
-      <c r="C3816" t="n">
-        <v>129.3</v>
-      </c>
-    </row>
-    <row r="3817">
-      <c r="A3817" s="2" t="n">
-        <v>46061.70833333334</v>
-      </c>
-      <c r="B3817" s="2" t="n">
-        <v>46061.75</v>
-      </c>
-      <c r="C3817" t="n">
-        <v>126.95</v>
-      </c>
-    </row>
-    <row r="3818">
-      <c r="A3818" s="2" t="n">
-        <v>46061.71875</v>
-      </c>
-      <c r="B3818" s="2" t="n">
-        <v>46061.76041666666</v>
-      </c>
-      <c r="C3818" t="n">
-        <v>129.89</v>
-      </c>
-    </row>
-    <row r="3819">
-      <c r="A3819" s="2" t="n">
-        <v>46061.72916666666</v>
-      </c>
-      <c r="B3819" s="2" t="n">
-        <v>46061.77083333334</v>
-      </c>
-      <c r="C3819" t="n">
-        <v>132.55</v>
-      </c>
-    </row>
-    <row r="3820">
-      <c r="A3820" s="2" t="n">
-        <v>46061.73958333334</v>
-      </c>
-      <c r="B3820" s="2" t="n">
-        <v>46061.78125</v>
-      </c>
-      <c r="C3820" t="n">
-        <v>129.84</v>
-      </c>
-    </row>
-    <row r="3821">
-      <c r="A3821" s="2" t="n">
-        <v>46061.75</v>
-      </c>
-      <c r="B3821" s="2" t="n">
-        <v>46061.79166666666</v>
-      </c>
-      <c r="C3821" t="n">
-        <v>132.96</v>
-      </c>
-    </row>
-    <row r="3822">
-      <c r="A3822" s="2" t="n">
-        <v>46061.76041666666</v>
-      </c>
-      <c r="B3822" s="2" t="n">
-        <v>46061.80208333334</v>
-      </c>
-      <c r="C3822" t="n">
-        <v>129.55</v>
-      </c>
-    </row>
-    <row r="3823">
-      <c r="A3823" s="2" t="n">
-        <v>46061.77083333334</v>
-      </c>
-      <c r="B3823" s="2" t="n">
-        <v>46061.8125</v>
-      </c>
-      <c r="C3823" t="n">
-        <v>125.09</v>
-      </c>
-    </row>
-    <row r="3824">
-      <c r="A3824" s="2" t="n">
-        <v>46061.78125</v>
-      </c>
-      <c r="B3824" s="2" t="n">
-        <v>46061.82291666666</v>
-      </c>
-      <c r="C3824" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3825">
-      <c r="A3825" s="2" t="n">
-        <v>46061.79166666666</v>
-      </c>
-      <c r="B3825" s="2" t="n">
-        <v>46061.83333333334</v>
-      </c>
-      <c r="C3825" t="n">
-        <v>122.21</v>
-      </c>
-    </row>
-    <row r="3826">
-      <c r="A3826" s="2" t="n">
-        <v>46061.80208333334</v>
-      </c>
-      <c r="B3826" s="2" t="n">
-        <v>46061.84375</v>
-      </c>
-      <c r="C3826" t="n">
-        <v>113.65</v>
-      </c>
-    </row>
-    <row r="3827">
-      <c r="A3827" s="2" t="n">
-        <v>46061.8125</v>
-      </c>
-      <c r="B3827" s="2" t="n">
-        <v>46061.85416666666</v>
-      </c>
-      <c r="C3827" t="n">
-        <v>109.35</v>
-      </c>
-    </row>
-    <row r="3828">
-      <c r="A3828" s="2" t="n">
-        <v>46061.82291666666</v>
-      </c>
-      <c r="B3828" s="2" t="n">
-        <v>46061.86458333334</v>
-      </c>
-      <c r="C3828" t="n">
-        <v>103.88</v>
-      </c>
-    </row>
-    <row r="3829">
-      <c r="A3829" s="2" t="n">
-        <v>46061.83333333334</v>
-      </c>
-      <c r="B3829" s="2" t="n">
-        <v>46061.875</v>
-      </c>
-      <c r="C3829" t="n">
-        <v>109.68</v>
-      </c>
-    </row>
-    <row r="3830">
-      <c r="A3830" s="2" t="n">
-        <v>46061.84375</v>
-      </c>
-      <c r="B3830" s="2" t="n">
-        <v>46061.88541666666</v>
-      </c>
-      <c r="C3830" t="n">
-        <v>107.09</v>
-      </c>
-    </row>
-    <row r="3831">
-      <c r="A3831" s="2" t="n">
-        <v>46061.85416666666</v>
-      </c>
-      <c r="B3831" s="2" t="n">
-        <v>46061.89583333334</v>
-      </c>
-      <c r="C3831" t="n">
-        <v>103.63</v>
-      </c>
-    </row>
-    <row r="3832">
-      <c r="A3832" s="2" t="n">
-        <v>46061.86458333334</v>
-      </c>
-      <c r="B3832" s="2" t="n">
-        <v>46061.90625</v>
-      </c>
-      <c r="C3832" t="n">
-        <v>101.05</v>
-      </c>
-    </row>
-    <row r="3833">
-      <c r="A3833" s="2" t="n">
-        <v>46061.875</v>
-      </c>
-      <c r="B3833" s="2" t="n">
-        <v>46061.91666666666</v>
-      </c>
-      <c r="C3833" t="n">
-        <v>105.51</v>
-      </c>
-    </row>
-    <row r="3834">
-      <c r="A3834" s="2" t="n">
-        <v>46061.88541666666</v>
-      </c>
-      <c r="B3834" s="2" t="n">
-        <v>46061.92708333334</v>
-      </c>
-      <c r="C3834" t="n">
-        <v>104.16</v>
-      </c>
-    </row>
-    <row r="3835">
-      <c r="A3835" s="2" t="n">
-        <v>46061.89583333334</v>
-      </c>
-      <c r="B3835" s="2" t="n">
-        <v>46061.9375</v>
-      </c>
-      <c r="C3835" t="n">
-        <v>104.14</v>
-      </c>
-    </row>
-    <row r="3836">
-      <c r="A3836" s="2" t="n">
-        <v>46061.90625</v>
-      </c>
-      <c r="B3836" s="2" t="n">
-        <v>46061.94791666666</v>
-      </c>
-      <c r="C3836" t="n">
-        <v>101.42</v>
-      </c>
-    </row>
-    <row r="3837">
-      <c r="A3837" s="2" t="n">
-        <v>46061.91666666666</v>
-      </c>
-      <c r="B3837" s="2" t="n">
-        <v>46061.95833333334</v>
-      </c>
-      <c r="C3837" t="n">
-        <v>102.25</v>
-      </c>
-    </row>
-    <row r="3838">
-      <c r="A3838" s="2" t="n">
-        <v>46061.92708333334</v>
-      </c>
-      <c r="B3838" s="2" t="n">
-        <v>46061.96875</v>
-      </c>
-      <c r="C3838" t="n">
-        <v>101.71</v>
-      </c>
-    </row>
-    <row r="3839">
-      <c r="A3839" s="2" t="n">
-        <v>46061.9375</v>
-      </c>
-      <c r="B3839" s="2" t="n">
-        <v>46061.97916666666</v>
-      </c>
-      <c r="C3839" t="n">
-        <v>100.28</v>
-      </c>
-    </row>
-    <row r="3840">
-      <c r="A3840" s="2" t="n">
-        <v>46061.94791666666</v>
-      </c>
-      <c r="B3840" s="2" t="n">
-        <v>46061.98958333334</v>
-      </c>
-      <c r="C3840" t="n">
-        <v>93.73999999999999</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update XLSX via API 09-02-2026, 14:07:16
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3744"/>
+  <dimension ref="A1:C3840"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41577,6 +41577,1062 @@
         <v>90.45999999999999</v>
       </c>
     </row>
+    <row r="3745">
+      <c r="A3745" s="2" t="n">
+        <v>46060.95833333334</v>
+      </c>
+      <c r="B3745" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="C3745" t="n">
+        <v>108.87</v>
+      </c>
+    </row>
+    <row r="3746">
+      <c r="A3746" s="2" t="n">
+        <v>46060.96875</v>
+      </c>
+      <c r="B3746" s="2" t="n">
+        <v>46061.01041666666</v>
+      </c>
+      <c r="C3746" t="n">
+        <v>101.13</v>
+      </c>
+    </row>
+    <row r="3747">
+      <c r="A3747" s="2" t="n">
+        <v>46060.97916666666</v>
+      </c>
+      <c r="B3747" s="2" t="n">
+        <v>46061.02083333334</v>
+      </c>
+      <c r="C3747" t="n">
+        <v>97.81999999999999</v>
+      </c>
+    </row>
+    <row r="3748">
+      <c r="A3748" s="2" t="n">
+        <v>46060.98958333334</v>
+      </c>
+      <c r="B3748" s="2" t="n">
+        <v>46061.03125</v>
+      </c>
+      <c r="C3748" t="n">
+        <v>93.06999999999999</v>
+      </c>
+    </row>
+    <row r="3749">
+      <c r="A3749" s="2" t="n">
+        <v>46061</v>
+      </c>
+      <c r="B3749" s="2" t="n">
+        <v>46061.04166666666</v>
+      </c>
+      <c r="C3749" t="n">
+        <v>97.79000000000001</v>
+      </c>
+    </row>
+    <row r="3750">
+      <c r="A3750" s="2" t="n">
+        <v>46061.01041666666</v>
+      </c>
+      <c r="B3750" s="2" t="n">
+        <v>46061.05208333334</v>
+      </c>
+      <c r="C3750" t="n">
+        <v>98.66</v>
+      </c>
+    </row>
+    <row r="3751">
+      <c r="A3751" s="2" t="n">
+        <v>46061.02083333334</v>
+      </c>
+      <c r="B3751" s="2" t="n">
+        <v>46061.0625</v>
+      </c>
+      <c r="C3751" t="n">
+        <v>97.09999999999999</v>
+      </c>
+    </row>
+    <row r="3752">
+      <c r="A3752" s="2" t="n">
+        <v>46061.03125</v>
+      </c>
+      <c r="B3752" s="2" t="n">
+        <v>46061.07291666666</v>
+      </c>
+      <c r="C3752" t="n">
+        <v>95.20999999999999</v>
+      </c>
+    </row>
+    <row r="3753">
+      <c r="A3753" s="2" t="n">
+        <v>46061.04166666666</v>
+      </c>
+      <c r="B3753" s="2" t="n">
+        <v>46061.08333333334</v>
+      </c>
+      <c r="C3753" t="n">
+        <v>98.05</v>
+      </c>
+    </row>
+    <row r="3754">
+      <c r="A3754" s="2" t="n">
+        <v>46061.05208333334</v>
+      </c>
+      <c r="B3754" s="2" t="n">
+        <v>46061.09375</v>
+      </c>
+      <c r="C3754" t="n">
+        <v>95.23</v>
+      </c>
+    </row>
+    <row r="3755">
+      <c r="A3755" s="2" t="n">
+        <v>46061.0625</v>
+      </c>
+      <c r="B3755" s="2" t="n">
+        <v>46061.10416666666</v>
+      </c>
+      <c r="C3755" t="n">
+        <v>92.69</v>
+      </c>
+    </row>
+    <row r="3756">
+      <c r="A3756" s="2" t="n">
+        <v>46061.07291666666</v>
+      </c>
+      <c r="B3756" s="2" t="n">
+        <v>46061.11458333334</v>
+      </c>
+      <c r="C3756" t="n">
+        <v>91.63</v>
+      </c>
+    </row>
+    <row r="3757">
+      <c r="A3757" s="2" t="n">
+        <v>46061.08333333334</v>
+      </c>
+      <c r="B3757" s="2" t="n">
+        <v>46061.125</v>
+      </c>
+      <c r="C3757" t="n">
+        <v>93.48999999999999</v>
+      </c>
+    </row>
+    <row r="3758">
+      <c r="A3758" s="2" t="n">
+        <v>46061.09375</v>
+      </c>
+      <c r="B3758" s="2" t="n">
+        <v>46061.13541666666</v>
+      </c>
+      <c r="C3758" t="n">
+        <v>92.25</v>
+      </c>
+    </row>
+    <row r="3759">
+      <c r="A3759" s="2" t="n">
+        <v>46061.10416666666</v>
+      </c>
+      <c r="B3759" s="2" t="n">
+        <v>46061.14583333334</v>
+      </c>
+      <c r="C3759" t="n">
+        <v>91.13</v>
+      </c>
+    </row>
+    <row r="3760">
+      <c r="A3760" s="2" t="n">
+        <v>46061.11458333334</v>
+      </c>
+      <c r="B3760" s="2" t="n">
+        <v>46061.15625</v>
+      </c>
+      <c r="C3760" t="n">
+        <v>91.61</v>
+      </c>
+    </row>
+    <row r="3761">
+      <c r="A3761" s="2" t="n">
+        <v>46061.125</v>
+      </c>
+      <c r="B3761" s="2" t="n">
+        <v>46061.16666666666</v>
+      </c>
+      <c r="C3761" t="n">
+        <v>90.34999999999999</v>
+      </c>
+    </row>
+    <row r="3762">
+      <c r="A3762" s="2" t="n">
+        <v>46061.13541666666</v>
+      </c>
+      <c r="B3762" s="2" t="n">
+        <v>46061.17708333334</v>
+      </c>
+      <c r="C3762" t="n">
+        <v>90.43000000000001</v>
+      </c>
+    </row>
+    <row r="3763">
+      <c r="A3763" s="2" t="n">
+        <v>46061.14583333334</v>
+      </c>
+      <c r="B3763" s="2" t="n">
+        <v>46061.1875</v>
+      </c>
+      <c r="C3763" t="n">
+        <v>90.73</v>
+      </c>
+    </row>
+    <row r="3764">
+      <c r="A3764" s="2" t="n">
+        <v>46061.15625</v>
+      </c>
+      <c r="B3764" s="2" t="n">
+        <v>46061.19791666666</v>
+      </c>
+      <c r="C3764" t="n">
+        <v>90.33</v>
+      </c>
+    </row>
+    <row r="3765">
+      <c r="A3765" s="2" t="n">
+        <v>46061.16666666666</v>
+      </c>
+      <c r="B3765" s="2" t="n">
+        <v>46061.20833333334</v>
+      </c>
+      <c r="C3765" t="n">
+        <v>92.12</v>
+      </c>
+    </row>
+    <row r="3766">
+      <c r="A3766" s="2" t="n">
+        <v>46061.17708333334</v>
+      </c>
+      <c r="B3766" s="2" t="n">
+        <v>46061.21875</v>
+      </c>
+      <c r="C3766" t="n">
+        <v>91.44</v>
+      </c>
+    </row>
+    <row r="3767">
+      <c r="A3767" s="2" t="n">
+        <v>46061.1875</v>
+      </c>
+      <c r="B3767" s="2" t="n">
+        <v>46061.22916666666</v>
+      </c>
+      <c r="C3767" t="n">
+        <v>90.36</v>
+      </c>
+    </row>
+    <row r="3768">
+      <c r="A3768" s="2" t="n">
+        <v>46061.19791666666</v>
+      </c>
+      <c r="B3768" s="2" t="n">
+        <v>46061.23958333334</v>
+      </c>
+      <c r="C3768" t="n">
+        <v>91.61</v>
+      </c>
+    </row>
+    <row r="3769">
+      <c r="A3769" s="2" t="n">
+        <v>46061.20833333334</v>
+      </c>
+      <c r="B3769" s="2" t="n">
+        <v>46061.25</v>
+      </c>
+      <c r="C3769" t="n">
+        <v>84.8</v>
+      </c>
+    </row>
+    <row r="3770">
+      <c r="A3770" s="2" t="n">
+        <v>46061.21875</v>
+      </c>
+      <c r="B3770" s="2" t="n">
+        <v>46061.26041666666</v>
+      </c>
+      <c r="C3770" t="n">
+        <v>87.67</v>
+      </c>
+    </row>
+    <row r="3771">
+      <c r="A3771" s="2" t="n">
+        <v>46061.22916666666</v>
+      </c>
+      <c r="B3771" s="2" t="n">
+        <v>46061.27083333334</v>
+      </c>
+      <c r="C3771" t="n">
+        <v>90.98</v>
+      </c>
+    </row>
+    <row r="3772">
+      <c r="A3772" s="2" t="n">
+        <v>46061.23958333334</v>
+      </c>
+      <c r="B3772" s="2" t="n">
+        <v>46061.28125</v>
+      </c>
+      <c r="C3772" t="n">
+        <v>95.95999999999999</v>
+      </c>
+    </row>
+    <row r="3773">
+      <c r="A3773" s="2" t="n">
+        <v>46061.25</v>
+      </c>
+      <c r="B3773" s="2" t="n">
+        <v>46061.29166666666</v>
+      </c>
+      <c r="C3773" t="n">
+        <v>88.2</v>
+      </c>
+    </row>
+    <row r="3774">
+      <c r="A3774" s="2" t="n">
+        <v>46061.26041666666</v>
+      </c>
+      <c r="B3774" s="2" t="n">
+        <v>46061.30208333334</v>
+      </c>
+      <c r="C3774" t="n">
+        <v>91.33</v>
+      </c>
+    </row>
+    <row r="3775">
+      <c r="A3775" s="2" t="n">
+        <v>46061.27083333334</v>
+      </c>
+      <c r="B3775" s="2" t="n">
+        <v>46061.3125</v>
+      </c>
+      <c r="C3775" t="n">
+        <v>94.69</v>
+      </c>
+    </row>
+    <row r="3776">
+      <c r="A3776" s="2" t="n">
+        <v>46061.28125</v>
+      </c>
+      <c r="B3776" s="2" t="n">
+        <v>46061.32291666666</v>
+      </c>
+      <c r="C3776" t="n">
+        <v>99.09999999999999</v>
+      </c>
+    </row>
+    <row r="3777">
+      <c r="A3777" s="2" t="n">
+        <v>46061.29166666666</v>
+      </c>
+      <c r="B3777" s="2" t="n">
+        <v>46061.33333333334</v>
+      </c>
+      <c r="C3777" t="n">
+        <v>94.41</v>
+      </c>
+    </row>
+    <row r="3778">
+      <c r="A3778" s="2" t="n">
+        <v>46061.30208333334</v>
+      </c>
+      <c r="B3778" s="2" t="n">
+        <v>46061.34375</v>
+      </c>
+      <c r="C3778" t="n">
+        <v>98.72</v>
+      </c>
+    </row>
+    <row r="3779">
+      <c r="A3779" s="2" t="n">
+        <v>46061.3125</v>
+      </c>
+      <c r="B3779" s="2" t="n">
+        <v>46061.35416666666</v>
+      </c>
+      <c r="C3779" t="n">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="3780">
+      <c r="A3780" s="2" t="n">
+        <v>46061.32291666666</v>
+      </c>
+      <c r="B3780" s="2" t="n">
+        <v>46061.36458333334</v>
+      </c>
+      <c r="C3780" t="n">
+        <v>100.04</v>
+      </c>
+    </row>
+    <row r="3781">
+      <c r="A3781" s="2" t="n">
+        <v>46061.33333333334</v>
+      </c>
+      <c r="B3781" s="2" t="n">
+        <v>46061.375</v>
+      </c>
+      <c r="C3781" t="n">
+        <v>100.16</v>
+      </c>
+    </row>
+    <row r="3782">
+      <c r="A3782" s="2" t="n">
+        <v>46061.34375</v>
+      </c>
+      <c r="B3782" s="2" t="n">
+        <v>46061.38541666666</v>
+      </c>
+      <c r="C3782" t="n">
+        <v>99.87</v>
+      </c>
+    </row>
+    <row r="3783">
+      <c r="A3783" s="2" t="n">
+        <v>46061.35416666666</v>
+      </c>
+      <c r="B3783" s="2" t="n">
+        <v>46061.39583333334</v>
+      </c>
+      <c r="C3783" t="n">
+        <v>99.48999999999999</v>
+      </c>
+    </row>
+    <row r="3784">
+      <c r="A3784" s="2" t="n">
+        <v>46061.36458333334</v>
+      </c>
+      <c r="B3784" s="2" t="n">
+        <v>46061.40625</v>
+      </c>
+      <c r="C3784" t="n">
+        <v>93.78</v>
+      </c>
+    </row>
+    <row r="3785">
+      <c r="A3785" s="2" t="n">
+        <v>46061.375</v>
+      </c>
+      <c r="B3785" s="2" t="n">
+        <v>46061.41666666666</v>
+      </c>
+      <c r="C3785" t="n">
+        <v>100.9</v>
+      </c>
+    </row>
+    <row r="3786">
+      <c r="A3786" s="2" t="n">
+        <v>46061.38541666666</v>
+      </c>
+      <c r="B3786" s="2" t="n">
+        <v>46061.42708333334</v>
+      </c>
+      <c r="C3786" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3787">
+      <c r="A3787" s="2" t="n">
+        <v>46061.39583333334</v>
+      </c>
+      <c r="B3787" s="2" t="n">
+        <v>46061.4375</v>
+      </c>
+      <c r="C3787" t="n">
+        <v>94.86</v>
+      </c>
+    </row>
+    <row r="3788">
+      <c r="A3788" s="2" t="n">
+        <v>46061.40625</v>
+      </c>
+      <c r="B3788" s="2" t="n">
+        <v>46061.44791666666</v>
+      </c>
+      <c r="C3788" t="n">
+        <v>93.12</v>
+      </c>
+    </row>
+    <row r="3789">
+      <c r="A3789" s="2" t="n">
+        <v>46061.41666666666</v>
+      </c>
+      <c r="B3789" s="2" t="n">
+        <v>46061.45833333334</v>
+      </c>
+      <c r="C3789" t="n">
+        <v>96.90000000000001</v>
+      </c>
+    </row>
+    <row r="3790">
+      <c r="A3790" s="2" t="n">
+        <v>46061.42708333334</v>
+      </c>
+      <c r="B3790" s="2" t="n">
+        <v>46061.46875</v>
+      </c>
+      <c r="C3790" t="n">
+        <v>93.98</v>
+      </c>
+    </row>
+    <row r="3791">
+      <c r="A3791" s="2" t="n">
+        <v>46061.4375</v>
+      </c>
+      <c r="B3791" s="2" t="n">
+        <v>46061.47916666666</v>
+      </c>
+      <c r="C3791" t="n">
+        <v>92.53</v>
+      </c>
+    </row>
+    <row r="3792">
+      <c r="A3792" s="2" t="n">
+        <v>46061.44791666666</v>
+      </c>
+      <c r="B3792" s="2" t="n">
+        <v>46061.48958333334</v>
+      </c>
+      <c r="C3792" t="n">
+        <v>90.44</v>
+      </c>
+    </row>
+    <row r="3793">
+      <c r="A3793" s="2" t="n">
+        <v>46061.45833333334</v>
+      </c>
+      <c r="B3793" s="2" t="n">
+        <v>46061.5</v>
+      </c>
+      <c r="C3793" t="n">
+        <v>92.03</v>
+      </c>
+    </row>
+    <row r="3794">
+      <c r="A3794" s="2" t="n">
+        <v>46061.46875</v>
+      </c>
+      <c r="B3794" s="2" t="n">
+        <v>46061.51041666666</v>
+      </c>
+      <c r="C3794" t="n">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="3795">
+      <c r="A3795" s="2" t="n">
+        <v>46061.47916666666</v>
+      </c>
+      <c r="B3795" s="2" t="n">
+        <v>46061.52083333334</v>
+      </c>
+      <c r="C3795" t="n">
+        <v>92.56</v>
+      </c>
+    </row>
+    <row r="3796">
+      <c r="A3796" s="2" t="n">
+        <v>46061.48958333334</v>
+      </c>
+      <c r="B3796" s="2" t="n">
+        <v>46061.53125</v>
+      </c>
+      <c r="C3796" t="n">
+        <v>89.59</v>
+      </c>
+    </row>
+    <row r="3797">
+      <c r="A3797" s="2" t="n">
+        <v>46061.5</v>
+      </c>
+      <c r="B3797" s="2" t="n">
+        <v>46061.54166666666</v>
+      </c>
+      <c r="C3797" t="n">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="3798">
+      <c r="A3798" s="2" t="n">
+        <v>46061.51041666666</v>
+      </c>
+      <c r="B3798" s="2" t="n">
+        <v>46061.55208333334</v>
+      </c>
+      <c r="C3798" t="n">
+        <v>88.97</v>
+      </c>
+    </row>
+    <row r="3799">
+      <c r="A3799" s="2" t="n">
+        <v>46061.52083333334</v>
+      </c>
+      <c r="B3799" s="2" t="n">
+        <v>46061.5625</v>
+      </c>
+      <c r="C3799" t="n">
+        <v>90.88</v>
+      </c>
+    </row>
+    <row r="3800">
+      <c r="A3800" s="2" t="n">
+        <v>46061.53125</v>
+      </c>
+      <c r="B3800" s="2" t="n">
+        <v>46061.57291666666</v>
+      </c>
+      <c r="C3800" t="n">
+        <v>89.17</v>
+      </c>
+    </row>
+    <row r="3801">
+      <c r="A3801" s="2" t="n">
+        <v>46061.54166666666</v>
+      </c>
+      <c r="B3801" s="2" t="n">
+        <v>46061.58333333334</v>
+      </c>
+      <c r="C3801" t="n">
+        <v>88.76000000000001</v>
+      </c>
+    </row>
+    <row r="3802">
+      <c r="A3802" s="2" t="n">
+        <v>46061.55208333334</v>
+      </c>
+      <c r="B3802" s="2" t="n">
+        <v>46061.59375</v>
+      </c>
+      <c r="C3802" t="n">
+        <v>89.90000000000001</v>
+      </c>
+    </row>
+    <row r="3803">
+      <c r="A3803" s="2" t="n">
+        <v>46061.5625</v>
+      </c>
+      <c r="B3803" s="2" t="n">
+        <v>46061.60416666666</v>
+      </c>
+      <c r="C3803" t="n">
+        <v>91.29000000000001</v>
+      </c>
+    </row>
+    <row r="3804">
+      <c r="A3804" s="2" t="n">
+        <v>46061.57291666666</v>
+      </c>
+      <c r="B3804" s="2" t="n">
+        <v>46061.61458333334</v>
+      </c>
+      <c r="C3804" t="n">
+        <v>93.73</v>
+      </c>
+    </row>
+    <row r="3805">
+      <c r="A3805" s="2" t="n">
+        <v>46061.58333333334</v>
+      </c>
+      <c r="B3805" s="2" t="n">
+        <v>46061.625</v>
+      </c>
+      <c r="C3805" t="n">
+        <v>92.69</v>
+      </c>
+    </row>
+    <row r="3806">
+      <c r="A3806" s="2" t="n">
+        <v>46061.59375</v>
+      </c>
+      <c r="B3806" s="2" t="n">
+        <v>46061.63541666666</v>
+      </c>
+      <c r="C3806" t="n">
+        <v>96.51000000000001</v>
+      </c>
+    </row>
+    <row r="3807">
+      <c r="A3807" s="2" t="n">
+        <v>46061.60416666666</v>
+      </c>
+      <c r="B3807" s="2" t="n">
+        <v>46061.64583333334</v>
+      </c>
+      <c r="C3807" t="n">
+        <v>99.09999999999999</v>
+      </c>
+    </row>
+    <row r="3808">
+      <c r="A3808" s="2" t="n">
+        <v>46061.61458333334</v>
+      </c>
+      <c r="B3808" s="2" t="n">
+        <v>46061.65625</v>
+      </c>
+      <c r="C3808" t="n">
+        <v>105.63</v>
+      </c>
+    </row>
+    <row r="3809">
+      <c r="A3809" s="2" t="n">
+        <v>46061.625</v>
+      </c>
+      <c r="B3809" s="2" t="n">
+        <v>46061.66666666666</v>
+      </c>
+      <c r="C3809" t="n">
+        <v>92.94</v>
+      </c>
+    </row>
+    <row r="3810">
+      <c r="A3810" s="2" t="n">
+        <v>46061.63541666666</v>
+      </c>
+      <c r="B3810" s="2" t="n">
+        <v>46061.67708333334</v>
+      </c>
+      <c r="C3810" t="n">
+        <v>100.57</v>
+      </c>
+    </row>
+    <row r="3811">
+      <c r="A3811" s="2" t="n">
+        <v>46061.64583333334</v>
+      </c>
+      <c r="B3811" s="2" t="n">
+        <v>46061.6875</v>
+      </c>
+      <c r="C3811" t="n">
+        <v>107.46</v>
+      </c>
+    </row>
+    <row r="3812">
+      <c r="A3812" s="2" t="n">
+        <v>46061.65625</v>
+      </c>
+      <c r="B3812" s="2" t="n">
+        <v>46061.69791666666</v>
+      </c>
+      <c r="C3812" t="n">
+        <v>118.19</v>
+      </c>
+    </row>
+    <row r="3813">
+      <c r="A3813" s="2" t="n">
+        <v>46061.66666666666</v>
+      </c>
+      <c r="B3813" s="2" t="n">
+        <v>46061.70833333334</v>
+      </c>
+      <c r="C3813" t="n">
+        <v>111.91</v>
+      </c>
+    </row>
+    <row r="3814">
+      <c r="A3814" s="2" t="n">
+        <v>46061.67708333334</v>
+      </c>
+      <c r="B3814" s="2" t="n">
+        <v>46061.71875</v>
+      </c>
+      <c r="C3814" t="n">
+        <v>120.09</v>
+      </c>
+    </row>
+    <row r="3815">
+      <c r="A3815" s="2" t="n">
+        <v>46061.6875</v>
+      </c>
+      <c r="B3815" s="2" t="n">
+        <v>46061.72916666666</v>
+      </c>
+      <c r="C3815" t="n">
+        <v>125.41</v>
+      </c>
+    </row>
+    <row r="3816">
+      <c r="A3816" s="2" t="n">
+        <v>46061.69791666666</v>
+      </c>
+      <c r="B3816" s="2" t="n">
+        <v>46061.73958333334</v>
+      </c>
+      <c r="C3816" t="n">
+        <v>129.3</v>
+      </c>
+    </row>
+    <row r="3817">
+      <c r="A3817" s="2" t="n">
+        <v>46061.70833333334</v>
+      </c>
+      <c r="B3817" s="2" t="n">
+        <v>46061.75</v>
+      </c>
+      <c r="C3817" t="n">
+        <v>126.95</v>
+      </c>
+    </row>
+    <row r="3818">
+      <c r="A3818" s="2" t="n">
+        <v>46061.71875</v>
+      </c>
+      <c r="B3818" s="2" t="n">
+        <v>46061.76041666666</v>
+      </c>
+      <c r="C3818" t="n">
+        <v>129.89</v>
+      </c>
+    </row>
+    <row r="3819">
+      <c r="A3819" s="2" t="n">
+        <v>46061.72916666666</v>
+      </c>
+      <c r="B3819" s="2" t="n">
+        <v>46061.77083333334</v>
+      </c>
+      <c r="C3819" t="n">
+        <v>132.55</v>
+      </c>
+    </row>
+    <row r="3820">
+      <c r="A3820" s="2" t="n">
+        <v>46061.73958333334</v>
+      </c>
+      <c r="B3820" s="2" t="n">
+        <v>46061.78125</v>
+      </c>
+      <c r="C3820" t="n">
+        <v>129.84</v>
+      </c>
+    </row>
+    <row r="3821">
+      <c r="A3821" s="2" t="n">
+        <v>46061.75</v>
+      </c>
+      <c r="B3821" s="2" t="n">
+        <v>46061.79166666666</v>
+      </c>
+      <c r="C3821" t="n">
+        <v>132.96</v>
+      </c>
+    </row>
+    <row r="3822">
+      <c r="A3822" s="2" t="n">
+        <v>46061.76041666666</v>
+      </c>
+      <c r="B3822" s="2" t="n">
+        <v>46061.80208333334</v>
+      </c>
+      <c r="C3822" t="n">
+        <v>129.55</v>
+      </c>
+    </row>
+    <row r="3823">
+      <c r="A3823" s="2" t="n">
+        <v>46061.77083333334</v>
+      </c>
+      <c r="B3823" s="2" t="n">
+        <v>46061.8125</v>
+      </c>
+      <c r="C3823" t="n">
+        <v>125.09</v>
+      </c>
+    </row>
+    <row r="3824">
+      <c r="A3824" s="2" t="n">
+        <v>46061.78125</v>
+      </c>
+      <c r="B3824" s="2" t="n">
+        <v>46061.82291666666</v>
+      </c>
+      <c r="C3824" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3825">
+      <c r="A3825" s="2" t="n">
+        <v>46061.79166666666</v>
+      </c>
+      <c r="B3825" s="2" t="n">
+        <v>46061.83333333334</v>
+      </c>
+      <c r="C3825" t="n">
+        <v>122.21</v>
+      </c>
+    </row>
+    <row r="3826">
+      <c r="A3826" s="2" t="n">
+        <v>46061.80208333334</v>
+      </c>
+      <c r="B3826" s="2" t="n">
+        <v>46061.84375</v>
+      </c>
+      <c r="C3826" t="n">
+        <v>113.65</v>
+      </c>
+    </row>
+    <row r="3827">
+      <c r="A3827" s="2" t="n">
+        <v>46061.8125</v>
+      </c>
+      <c r="B3827" s="2" t="n">
+        <v>46061.85416666666</v>
+      </c>
+      <c r="C3827" t="n">
+        <v>109.35</v>
+      </c>
+    </row>
+    <row r="3828">
+      <c r="A3828" s="2" t="n">
+        <v>46061.82291666666</v>
+      </c>
+      <c r="B3828" s="2" t="n">
+        <v>46061.86458333334</v>
+      </c>
+      <c r="C3828" t="n">
+        <v>103.88</v>
+      </c>
+    </row>
+    <row r="3829">
+      <c r="A3829" s="2" t="n">
+        <v>46061.83333333334</v>
+      </c>
+      <c r="B3829" s="2" t="n">
+        <v>46061.875</v>
+      </c>
+      <c r="C3829" t="n">
+        <v>109.68</v>
+      </c>
+    </row>
+    <row r="3830">
+      <c r="A3830" s="2" t="n">
+        <v>46061.84375</v>
+      </c>
+      <c r="B3830" s="2" t="n">
+        <v>46061.88541666666</v>
+      </c>
+      <c r="C3830" t="n">
+        <v>107.09</v>
+      </c>
+    </row>
+    <row r="3831">
+      <c r="A3831" s="2" t="n">
+        <v>46061.85416666666</v>
+      </c>
+      <c r="B3831" s="2" t="n">
+        <v>46061.89583333334</v>
+      </c>
+      <c r="C3831" t="n">
+        <v>103.63</v>
+      </c>
+    </row>
+    <row r="3832">
+      <c r="A3832" s="2" t="n">
+        <v>46061.86458333334</v>
+      </c>
+      <c r="B3832" s="2" t="n">
+        <v>46061.90625</v>
+      </c>
+      <c r="C3832" t="n">
+        <v>101.05</v>
+      </c>
+    </row>
+    <row r="3833">
+      <c r="A3833" s="2" t="n">
+        <v>46061.875</v>
+      </c>
+      <c r="B3833" s="2" t="n">
+        <v>46061.91666666666</v>
+      </c>
+      <c r="C3833" t="n">
+        <v>105.51</v>
+      </c>
+    </row>
+    <row r="3834">
+      <c r="A3834" s="2" t="n">
+        <v>46061.88541666666</v>
+      </c>
+      <c r="B3834" s="2" t="n">
+        <v>46061.92708333334</v>
+      </c>
+      <c r="C3834" t="n">
+        <v>104.16</v>
+      </c>
+    </row>
+    <row r="3835">
+      <c r="A3835" s="2" t="n">
+        <v>46061.89583333334</v>
+      </c>
+      <c r="B3835" s="2" t="n">
+        <v>46061.9375</v>
+      </c>
+      <c r="C3835" t="n">
+        <v>104.14</v>
+      </c>
+    </row>
+    <row r="3836">
+      <c r="A3836" s="2" t="n">
+        <v>46061.90625</v>
+      </c>
+      <c r="B3836" s="2" t="n">
+        <v>46061.94791666666</v>
+      </c>
+      <c r="C3836" t="n">
+        <v>101.42</v>
+      </c>
+    </row>
+    <row r="3837">
+      <c r="A3837" s="2" t="n">
+        <v>46061.91666666666</v>
+      </c>
+      <c r="B3837" s="2" t="n">
+        <v>46061.95833333334</v>
+      </c>
+      <c r="C3837" t="n">
+        <v>102.25</v>
+      </c>
+    </row>
+    <row r="3838">
+      <c r="A3838" s="2" t="n">
+        <v>46061.92708333334</v>
+      </c>
+      <c r="B3838" s="2" t="n">
+        <v>46061.96875</v>
+      </c>
+      <c r="C3838" t="n">
+        <v>101.71</v>
+      </c>
+    </row>
+    <row r="3839">
+      <c r="A3839" s="2" t="n">
+        <v>46061.9375</v>
+      </c>
+      <c r="B3839" s="2" t="n">
+        <v>46061.97916666666</v>
+      </c>
+      <c r="C3839" t="n">
+        <v>100.28</v>
+      </c>
+    </row>
+    <row r="3840">
+      <c r="A3840" s="2" t="n">
+        <v>46061.94791666666</v>
+      </c>
+      <c r="B3840" s="2" t="n">
+        <v>46061.98958333334</v>
+      </c>
+      <c r="C3840" t="n">
+        <v>93.73999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update XLSX via API 09-02-2026, 14:21:39
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -41579,1058 +41579,1058 @@
     </row>
     <row r="3745">
       <c r="A3745" s="2" t="n">
-        <v>46060.95833333334</v>
+        <v>46061.95833333334</v>
       </c>
       <c r="B3745" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="C3745" t="n">
-        <v>108.87</v>
+        <v>99.88</v>
       </c>
     </row>
     <row r="3746">
       <c r="A3746" s="2" t="n">
-        <v>46060.96875</v>
+        <v>46061.96875</v>
       </c>
       <c r="B3746" s="2" t="n">
-        <v>46061.01041666666</v>
+        <v>46062.01041666666</v>
       </c>
       <c r="C3746" t="n">
-        <v>101.13</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="3747">
       <c r="A3747" s="2" t="n">
-        <v>46060.97916666666</v>
+        <v>46061.97916666666</v>
       </c>
       <c r="B3747" s="2" t="n">
-        <v>46061.02083333334</v>
+        <v>46062.02083333334</v>
       </c>
       <c r="C3747" t="n">
-        <v>97.81999999999999</v>
+        <v>92.38</v>
       </c>
     </row>
     <row r="3748">
       <c r="A3748" s="2" t="n">
-        <v>46060.98958333334</v>
+        <v>46061.98958333334</v>
       </c>
       <c r="B3748" s="2" t="n">
-        <v>46061.03125</v>
+        <v>46062.03125</v>
       </c>
       <c r="C3748" t="n">
-        <v>93.06999999999999</v>
+        <v>89.40000000000001</v>
       </c>
     </row>
     <row r="3749">
       <c r="A3749" s="2" t="n">
-        <v>46061</v>
+        <v>46062</v>
       </c>
       <c r="B3749" s="2" t="n">
-        <v>46061.04166666666</v>
+        <v>46062.04166666666</v>
       </c>
       <c r="C3749" t="n">
-        <v>97.79000000000001</v>
+        <v>95.92</v>
       </c>
     </row>
     <row r="3750">
       <c r="A3750" s="2" t="n">
-        <v>46061.01041666666</v>
+        <v>46062.01041666666</v>
       </c>
       <c r="B3750" s="2" t="n">
-        <v>46061.05208333334</v>
+        <v>46062.05208333334</v>
       </c>
       <c r="C3750" t="n">
-        <v>98.66</v>
+        <v>93.2</v>
       </c>
     </row>
     <row r="3751">
       <c r="A3751" s="2" t="n">
-        <v>46061.02083333334</v>
+        <v>46062.02083333334</v>
       </c>
       <c r="B3751" s="2" t="n">
-        <v>46061.0625</v>
+        <v>46062.0625</v>
       </c>
       <c r="C3751" t="n">
-        <v>97.09999999999999</v>
+        <v>92.94</v>
       </c>
     </row>
     <row r="3752">
       <c r="A3752" s="2" t="n">
-        <v>46061.03125</v>
+        <v>46062.03125</v>
       </c>
       <c r="B3752" s="2" t="n">
-        <v>46061.07291666666</v>
+        <v>46062.07291666666</v>
       </c>
       <c r="C3752" t="n">
-        <v>95.20999999999999</v>
+        <v>90.53</v>
       </c>
     </row>
     <row r="3753">
       <c r="A3753" s="2" t="n">
-        <v>46061.04166666666</v>
+        <v>46062.04166666666</v>
       </c>
       <c r="B3753" s="2" t="n">
-        <v>46061.08333333334</v>
+        <v>46062.08333333334</v>
       </c>
       <c r="C3753" t="n">
-        <v>98.05</v>
+        <v>94.06999999999999</v>
       </c>
     </row>
     <row r="3754">
       <c r="A3754" s="2" t="n">
-        <v>46061.05208333334</v>
+        <v>46062.05208333334</v>
       </c>
       <c r="B3754" s="2" t="n">
-        <v>46061.09375</v>
+        <v>46062.09375</v>
       </c>
       <c r="C3754" t="n">
-        <v>95.23</v>
+        <v>92.25</v>
       </c>
     </row>
     <row r="3755">
       <c r="A3755" s="2" t="n">
-        <v>46061.0625</v>
+        <v>46062.0625</v>
       </c>
       <c r="B3755" s="2" t="n">
-        <v>46061.10416666666</v>
+        <v>46062.10416666666</v>
       </c>
       <c r="C3755" t="n">
-        <v>92.69</v>
+        <v>92.75</v>
       </c>
     </row>
     <row r="3756">
       <c r="A3756" s="2" t="n">
-        <v>46061.07291666666</v>
+        <v>46062.07291666666</v>
       </c>
       <c r="B3756" s="2" t="n">
-        <v>46061.11458333334</v>
+        <v>46062.11458333334</v>
       </c>
       <c r="C3756" t="n">
-        <v>91.63</v>
+        <v>88.92</v>
       </c>
     </row>
     <row r="3757">
       <c r="A3757" s="2" t="n">
-        <v>46061.08333333334</v>
+        <v>46062.08333333334</v>
       </c>
       <c r="B3757" s="2" t="n">
-        <v>46061.125</v>
+        <v>46062.125</v>
       </c>
       <c r="C3757" t="n">
-        <v>93.48999999999999</v>
+        <v>90.94</v>
       </c>
     </row>
     <row r="3758">
       <c r="A3758" s="2" t="n">
-        <v>46061.09375</v>
+        <v>46062.09375</v>
       </c>
       <c r="B3758" s="2" t="n">
-        <v>46061.13541666666</v>
+        <v>46062.13541666666</v>
       </c>
       <c r="C3758" t="n">
-        <v>92.25</v>
+        <v>90.03</v>
       </c>
     </row>
     <row r="3759">
       <c r="A3759" s="2" t="n">
-        <v>46061.10416666666</v>
+        <v>46062.10416666666</v>
       </c>
       <c r="B3759" s="2" t="n">
-        <v>46061.14583333334</v>
+        <v>46062.14583333334</v>
       </c>
       <c r="C3759" t="n">
-        <v>91.13</v>
+        <v>90.25</v>
       </c>
     </row>
     <row r="3760">
       <c r="A3760" s="2" t="n">
-        <v>46061.11458333334</v>
+        <v>46062.11458333334</v>
       </c>
       <c r="B3760" s="2" t="n">
-        <v>46061.15625</v>
+        <v>46062.15625</v>
       </c>
       <c r="C3760" t="n">
-        <v>91.61</v>
+        <v>89.77</v>
       </c>
     </row>
     <row r="3761">
       <c r="A3761" s="2" t="n">
-        <v>46061.125</v>
+        <v>46062.125</v>
       </c>
       <c r="B3761" s="2" t="n">
-        <v>46061.16666666666</v>
+        <v>46062.16666666666</v>
       </c>
       <c r="C3761" t="n">
-        <v>90.34999999999999</v>
+        <v>87.87</v>
       </c>
     </row>
     <row r="3762">
       <c r="A3762" s="2" t="n">
-        <v>46061.13541666666</v>
+        <v>46062.13541666666</v>
       </c>
       <c r="B3762" s="2" t="n">
-        <v>46061.17708333334</v>
+        <v>46062.17708333334</v>
       </c>
       <c r="C3762" t="n">
-        <v>90.43000000000001</v>
+        <v>89.18000000000001</v>
       </c>
     </row>
     <row r="3763">
       <c r="A3763" s="2" t="n">
-        <v>46061.14583333334</v>
+        <v>46062.14583333334</v>
       </c>
       <c r="B3763" s="2" t="n">
-        <v>46061.1875</v>
+        <v>46062.1875</v>
       </c>
       <c r="C3763" t="n">
-        <v>90.73</v>
+        <v>90.11</v>
       </c>
     </row>
     <row r="3764">
       <c r="A3764" s="2" t="n">
-        <v>46061.15625</v>
+        <v>46062.15625</v>
       </c>
       <c r="B3764" s="2" t="n">
-        <v>46061.19791666666</v>
+        <v>46062.19791666666</v>
       </c>
       <c r="C3764" t="n">
-        <v>90.33</v>
+        <v>95.18000000000001</v>
       </c>
     </row>
     <row r="3765">
       <c r="A3765" s="2" t="n">
-        <v>46061.16666666666</v>
+        <v>46062.16666666666</v>
       </c>
       <c r="B3765" s="2" t="n">
-        <v>46061.20833333334</v>
+        <v>46062.20833333334</v>
       </c>
       <c r="C3765" t="n">
-        <v>92.12</v>
+        <v>91.87</v>
       </c>
     </row>
     <row r="3766">
       <c r="A3766" s="2" t="n">
-        <v>46061.17708333334</v>
+        <v>46062.17708333334</v>
       </c>
       <c r="B3766" s="2" t="n">
-        <v>46061.21875</v>
+        <v>46062.21875</v>
       </c>
       <c r="C3766" t="n">
-        <v>91.44</v>
+        <v>96.48</v>
       </c>
     </row>
     <row r="3767">
       <c r="A3767" s="2" t="n">
-        <v>46061.1875</v>
+        <v>46062.1875</v>
       </c>
       <c r="B3767" s="2" t="n">
-        <v>46061.22916666666</v>
+        <v>46062.22916666666</v>
       </c>
       <c r="C3767" t="n">
-        <v>90.36</v>
+        <v>101.27</v>
       </c>
     </row>
     <row r="3768">
       <c r="A3768" s="2" t="n">
-        <v>46061.19791666666</v>
+        <v>46062.19791666666</v>
       </c>
       <c r="B3768" s="2" t="n">
-        <v>46061.23958333334</v>
+        <v>46062.23958333334</v>
       </c>
       <c r="C3768" t="n">
-        <v>91.61</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3769">
       <c r="A3769" s="2" t="n">
-        <v>46061.20833333334</v>
+        <v>46062.20833333334</v>
       </c>
       <c r="B3769" s="2" t="n">
-        <v>46061.25</v>
+        <v>46062.25</v>
       </c>
       <c r="C3769" t="n">
-        <v>84.8</v>
+        <v>101.27</v>
       </c>
     </row>
     <row r="3770">
       <c r="A3770" s="2" t="n">
-        <v>46061.21875</v>
+        <v>46062.21875</v>
       </c>
       <c r="B3770" s="2" t="n">
-        <v>46061.26041666666</v>
+        <v>46062.26041666666</v>
       </c>
       <c r="C3770" t="n">
-        <v>87.67</v>
+        <v>116.41</v>
       </c>
     </row>
     <row r="3771">
       <c r="A3771" s="2" t="n">
-        <v>46061.22916666666</v>
+        <v>46062.22916666666</v>
       </c>
       <c r="B3771" s="2" t="n">
-        <v>46061.27083333334</v>
+        <v>46062.27083333334</v>
       </c>
       <c r="C3771" t="n">
-        <v>90.98</v>
+        <v>130.75</v>
       </c>
     </row>
     <row r="3772">
       <c r="A3772" s="2" t="n">
-        <v>46061.23958333334</v>
+        <v>46062.23958333334</v>
       </c>
       <c r="B3772" s="2" t="n">
-        <v>46061.28125</v>
+        <v>46062.28125</v>
       </c>
       <c r="C3772" t="n">
-        <v>95.95999999999999</v>
+        <v>158.33</v>
       </c>
     </row>
     <row r="3773">
       <c r="A3773" s="2" t="n">
-        <v>46061.25</v>
+        <v>46062.25</v>
       </c>
       <c r="B3773" s="2" t="n">
-        <v>46061.29166666666</v>
+        <v>46062.29166666666</v>
       </c>
       <c r="C3773" t="n">
-        <v>88.2</v>
+        <v>129.99</v>
       </c>
     </row>
     <row r="3774">
       <c r="A3774" s="2" t="n">
-        <v>46061.26041666666</v>
+        <v>46062.26041666666</v>
       </c>
       <c r="B3774" s="2" t="n">
-        <v>46061.30208333334</v>
+        <v>46062.30208333334</v>
       </c>
       <c r="C3774" t="n">
-        <v>91.33</v>
+        <v>152.36</v>
       </c>
     </row>
     <row r="3775">
       <c r="A3775" s="2" t="n">
-        <v>46061.27083333334</v>
+        <v>46062.27083333334</v>
       </c>
       <c r="B3775" s="2" t="n">
-        <v>46061.3125</v>
+        <v>46062.3125</v>
       </c>
       <c r="C3775" t="n">
-        <v>94.69</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3776">
       <c r="A3776" s="2" t="n">
-        <v>46061.28125</v>
+        <v>46062.28125</v>
       </c>
       <c r="B3776" s="2" t="n">
-        <v>46061.32291666666</v>
+        <v>46062.32291666666</v>
       </c>
       <c r="C3776" t="n">
-        <v>99.09999999999999</v>
+        <v>163.64</v>
       </c>
     </row>
     <row r="3777">
       <c r="A3777" s="2" t="n">
-        <v>46061.29166666666</v>
+        <v>46062.29166666666</v>
       </c>
       <c r="B3777" s="2" t="n">
-        <v>46061.33333333334</v>
+        <v>46062.33333333334</v>
       </c>
       <c r="C3777" t="n">
-        <v>94.41</v>
+        <v>170.29</v>
       </c>
     </row>
     <row r="3778">
       <c r="A3778" s="2" t="n">
-        <v>46061.30208333334</v>
+        <v>46062.30208333334</v>
       </c>
       <c r="B3778" s="2" t="n">
-        <v>46061.34375</v>
+        <v>46062.34375</v>
       </c>
       <c r="C3778" t="n">
-        <v>98.72</v>
+        <v>179.32</v>
       </c>
     </row>
     <row r="3779">
       <c r="A3779" s="2" t="n">
-        <v>46061.3125</v>
+        <v>46062.3125</v>
       </c>
       <c r="B3779" s="2" t="n">
-        <v>46061.35416666666</v>
+        <v>46062.35416666666</v>
       </c>
       <c r="C3779" t="n">
-        <v>100.1</v>
+        <v>179.34</v>
       </c>
     </row>
     <row r="3780">
       <c r="A3780" s="2" t="n">
-        <v>46061.32291666666</v>
+        <v>46062.32291666666</v>
       </c>
       <c r="B3780" s="2" t="n">
-        <v>46061.36458333334</v>
+        <v>46062.36458333334</v>
       </c>
       <c r="C3780" t="n">
-        <v>100.04</v>
+        <v>175.09</v>
       </c>
     </row>
     <row r="3781">
       <c r="A3781" s="2" t="n">
-        <v>46061.33333333334</v>
+        <v>46062.33333333334</v>
       </c>
       <c r="B3781" s="2" t="n">
-        <v>46061.375</v>
+        <v>46062.375</v>
       </c>
       <c r="C3781" t="n">
-        <v>100.16</v>
+        <v>182.41</v>
       </c>
     </row>
     <row r="3782">
       <c r="A3782" s="2" t="n">
-        <v>46061.34375</v>
+        <v>46062.34375</v>
       </c>
       <c r="B3782" s="2" t="n">
-        <v>46061.38541666666</v>
+        <v>46062.38541666666</v>
       </c>
       <c r="C3782" t="n">
-        <v>99.87</v>
+        <v>171.32</v>
       </c>
     </row>
     <row r="3783">
       <c r="A3783" s="2" t="n">
-        <v>46061.35416666666</v>
+        <v>46062.35416666666</v>
       </c>
       <c r="B3783" s="2" t="n">
-        <v>46061.39583333334</v>
+        <v>46062.39583333334</v>
       </c>
       <c r="C3783" t="n">
-        <v>99.48999999999999</v>
+        <v>151.84</v>
       </c>
     </row>
     <row r="3784">
       <c r="A3784" s="2" t="n">
-        <v>46061.36458333334</v>
+        <v>46062.36458333334</v>
       </c>
       <c r="B3784" s="2" t="n">
-        <v>46061.40625</v>
+        <v>46062.40625</v>
       </c>
       <c r="C3784" t="n">
-        <v>93.78</v>
+        <v>148.06</v>
       </c>
     </row>
     <row r="3785">
       <c r="A3785" s="2" t="n">
-        <v>46061.375</v>
+        <v>46062.375</v>
       </c>
       <c r="B3785" s="2" t="n">
-        <v>46061.41666666666</v>
+        <v>46062.41666666666</v>
       </c>
       <c r="C3785" t="n">
-        <v>100.9</v>
+        <v>158.59</v>
       </c>
     </row>
     <row r="3786">
       <c r="A3786" s="2" t="n">
-        <v>46061.38541666666</v>
+        <v>46062.38541666666</v>
       </c>
       <c r="B3786" s="2" t="n">
-        <v>46061.42708333334</v>
+        <v>46062.42708333334</v>
       </c>
       <c r="C3786" t="n">
-        <v>98</v>
+        <v>154.96</v>
       </c>
     </row>
     <row r="3787">
       <c r="A3787" s="2" t="n">
-        <v>46061.39583333334</v>
+        <v>46062.39583333334</v>
       </c>
       <c r="B3787" s="2" t="n">
-        <v>46061.4375</v>
+        <v>46062.4375</v>
       </c>
       <c r="C3787" t="n">
-        <v>94.86</v>
+        <v>146.04</v>
       </c>
     </row>
     <row r="3788">
       <c r="A3788" s="2" t="n">
-        <v>46061.40625</v>
+        <v>46062.40625</v>
       </c>
       <c r="B3788" s="2" t="n">
-        <v>46061.44791666666</v>
+        <v>46062.44791666666</v>
       </c>
       <c r="C3788" t="n">
-        <v>93.12</v>
+        <v>136.63</v>
       </c>
     </row>
     <row r="3789">
       <c r="A3789" s="2" t="n">
-        <v>46061.41666666666</v>
+        <v>46062.41666666666</v>
       </c>
       <c r="B3789" s="2" t="n">
-        <v>46061.45833333334</v>
+        <v>46062.45833333334</v>
       </c>
       <c r="C3789" t="n">
-        <v>96.90000000000001</v>
+        <v>142.94</v>
       </c>
     </row>
     <row r="3790">
       <c r="A3790" s="2" t="n">
-        <v>46061.42708333334</v>
+        <v>46062.42708333334</v>
       </c>
       <c r="B3790" s="2" t="n">
-        <v>46061.46875</v>
+        <v>46062.46875</v>
       </c>
       <c r="C3790" t="n">
-        <v>93.98</v>
+        <v>138.97</v>
       </c>
     </row>
     <row r="3791">
       <c r="A3791" s="2" t="n">
-        <v>46061.4375</v>
+        <v>46062.4375</v>
       </c>
       <c r="B3791" s="2" t="n">
-        <v>46061.47916666666</v>
+        <v>46062.47916666666</v>
       </c>
       <c r="C3791" t="n">
-        <v>92.53</v>
+        <v>136.31</v>
       </c>
     </row>
     <row r="3792">
       <c r="A3792" s="2" t="n">
-        <v>46061.44791666666</v>
+        <v>46062.44791666666</v>
       </c>
       <c r="B3792" s="2" t="n">
-        <v>46061.48958333334</v>
+        <v>46062.48958333334</v>
       </c>
       <c r="C3792" t="n">
-        <v>90.44</v>
+        <v>129.95</v>
       </c>
     </row>
     <row r="3793">
       <c r="A3793" s="2" t="n">
-        <v>46061.45833333334</v>
+        <v>46062.45833333334</v>
       </c>
       <c r="B3793" s="2" t="n">
-        <v>46061.5</v>
+        <v>46062.5</v>
       </c>
       <c r="C3793" t="n">
-        <v>92.03</v>
+        <v>138.44</v>
       </c>
     </row>
     <row r="3794">
       <c r="A3794" s="2" t="n">
-        <v>46061.46875</v>
+        <v>46062.46875</v>
       </c>
       <c r="B3794" s="2" t="n">
-        <v>46061.51041666666</v>
+        <v>46062.51041666666</v>
       </c>
       <c r="C3794" t="n">
-        <v>90.5</v>
+        <v>131.46</v>
       </c>
     </row>
     <row r="3795">
       <c r="A3795" s="2" t="n">
-        <v>46061.47916666666</v>
+        <v>46062.47916666666</v>
       </c>
       <c r="B3795" s="2" t="n">
-        <v>46061.52083333334</v>
+        <v>46062.52083333334</v>
       </c>
       <c r="C3795" t="n">
-        <v>92.56</v>
+        <v>129.11</v>
       </c>
     </row>
     <row r="3796">
       <c r="A3796" s="2" t="n">
-        <v>46061.48958333334</v>
+        <v>46062.48958333334</v>
       </c>
       <c r="B3796" s="2" t="n">
-        <v>46061.53125</v>
+        <v>46062.53125</v>
       </c>
       <c r="C3796" t="n">
-        <v>89.59</v>
+        <v>122.74</v>
       </c>
     </row>
     <row r="3797">
       <c r="A3797" s="2" t="n">
-        <v>46061.5</v>
+        <v>46062.5</v>
       </c>
       <c r="B3797" s="2" t="n">
-        <v>46061.54166666666</v>
+        <v>46062.54166666666</v>
       </c>
       <c r="C3797" t="n">
-        <v>90.8</v>
+        <v>130.01</v>
       </c>
     </row>
     <row r="3798">
       <c r="A3798" s="2" t="n">
-        <v>46061.51041666666</v>
+        <v>46062.51041666666</v>
       </c>
       <c r="B3798" s="2" t="n">
-        <v>46061.55208333334</v>
+        <v>46062.55208333334</v>
       </c>
       <c r="C3798" t="n">
-        <v>88.97</v>
+        <v>128.36</v>
       </c>
     </row>
     <row r="3799">
       <c r="A3799" s="2" t="n">
-        <v>46061.52083333334</v>
+        <v>46062.52083333334</v>
       </c>
       <c r="B3799" s="2" t="n">
-        <v>46061.5625</v>
+        <v>46062.5625</v>
       </c>
       <c r="C3799" t="n">
-        <v>90.88</v>
+        <v>124.6</v>
       </c>
     </row>
     <row r="3800">
       <c r="A3800" s="2" t="n">
-        <v>46061.53125</v>
+        <v>46062.53125</v>
       </c>
       <c r="B3800" s="2" t="n">
-        <v>46061.57291666666</v>
+        <v>46062.57291666666</v>
       </c>
       <c r="C3800" t="n">
-        <v>89.17</v>
+        <v>120.26</v>
       </c>
     </row>
     <row r="3801">
       <c r="A3801" s="2" t="n">
-        <v>46061.54166666666</v>
+        <v>46062.54166666666</v>
       </c>
       <c r="B3801" s="2" t="n">
-        <v>46061.58333333334</v>
+        <v>46062.58333333334</v>
       </c>
       <c r="C3801" t="n">
-        <v>88.76000000000001</v>
+        <v>116.47</v>
       </c>
     </row>
     <row r="3802">
       <c r="A3802" s="2" t="n">
-        <v>46061.55208333334</v>
+        <v>46062.55208333334</v>
       </c>
       <c r="B3802" s="2" t="n">
-        <v>46061.59375</v>
+        <v>46062.59375</v>
       </c>
       <c r="C3802" t="n">
-        <v>89.90000000000001</v>
+        <v>125.23</v>
       </c>
     </row>
     <row r="3803">
       <c r="A3803" s="2" t="n">
-        <v>46061.5625</v>
+        <v>46062.5625</v>
       </c>
       <c r="B3803" s="2" t="n">
-        <v>46061.60416666666</v>
+        <v>46062.60416666666</v>
       </c>
       <c r="C3803" t="n">
-        <v>91.29000000000001</v>
+        <v>132.18</v>
       </c>
     </row>
     <row r="3804">
       <c r="A3804" s="2" t="n">
-        <v>46061.57291666666</v>
+        <v>46062.57291666666</v>
       </c>
       <c r="B3804" s="2" t="n">
-        <v>46061.61458333334</v>
+        <v>46062.61458333334</v>
       </c>
       <c r="C3804" t="n">
-        <v>93.73</v>
+        <v>140.5</v>
       </c>
     </row>
     <row r="3805">
       <c r="A3805" s="2" t="n">
-        <v>46061.58333333334</v>
+        <v>46062.58333333334</v>
       </c>
       <c r="B3805" s="2" t="n">
-        <v>46061.625</v>
+        <v>46062.625</v>
       </c>
       <c r="C3805" t="n">
-        <v>92.69</v>
+        <v>120.08</v>
       </c>
     </row>
     <row r="3806">
       <c r="A3806" s="2" t="n">
-        <v>46061.59375</v>
+        <v>46062.59375</v>
       </c>
       <c r="B3806" s="2" t="n">
-        <v>46061.63541666666</v>
+        <v>46062.63541666666</v>
       </c>
       <c r="C3806" t="n">
-        <v>96.51000000000001</v>
+        <v>129.9</v>
       </c>
     </row>
     <row r="3807">
       <c r="A3807" s="2" t="n">
-        <v>46061.60416666666</v>
+        <v>46062.60416666666</v>
       </c>
       <c r="B3807" s="2" t="n">
-        <v>46061.64583333334</v>
+        <v>46062.64583333334</v>
       </c>
       <c r="C3807" t="n">
-        <v>99.09999999999999</v>
+        <v>145.32</v>
       </c>
     </row>
     <row r="3808">
       <c r="A3808" s="2" t="n">
-        <v>46061.61458333334</v>
+        <v>46062.61458333334</v>
       </c>
       <c r="B3808" s="2" t="n">
-        <v>46061.65625</v>
+        <v>46062.65625</v>
       </c>
       <c r="C3808" t="n">
-        <v>105.63</v>
+        <v>157.91</v>
       </c>
     </row>
     <row r="3809">
       <c r="A3809" s="2" t="n">
-        <v>46061.625</v>
+        <v>46062.625</v>
       </c>
       <c r="B3809" s="2" t="n">
-        <v>46061.66666666666</v>
+        <v>46062.66666666666</v>
       </c>
       <c r="C3809" t="n">
-        <v>92.94</v>
+        <v>128.61</v>
       </c>
     </row>
     <row r="3810">
       <c r="A3810" s="2" t="n">
-        <v>46061.63541666666</v>
+        <v>46062.63541666666</v>
       </c>
       <c r="B3810" s="2" t="n">
-        <v>46061.67708333334</v>
+        <v>46062.67708333334</v>
       </c>
       <c r="C3810" t="n">
-        <v>100.57</v>
+        <v>148.24</v>
       </c>
     </row>
     <row r="3811">
       <c r="A3811" s="2" t="n">
-        <v>46061.64583333334</v>
+        <v>46062.64583333334</v>
       </c>
       <c r="B3811" s="2" t="n">
-        <v>46061.6875</v>
+        <v>46062.6875</v>
       </c>
       <c r="C3811" t="n">
-        <v>107.46</v>
+        <v>168.24</v>
       </c>
     </row>
     <row r="3812">
       <c r="A3812" s="2" t="n">
-        <v>46061.65625</v>
+        <v>46062.65625</v>
       </c>
       <c r="B3812" s="2" t="n">
-        <v>46061.69791666666</v>
+        <v>46062.69791666666</v>
       </c>
       <c r="C3812" t="n">
-        <v>118.19</v>
+        <v>175.4</v>
       </c>
     </row>
     <row r="3813">
       <c r="A3813" s="2" t="n">
-        <v>46061.66666666666</v>
+        <v>46062.66666666666</v>
       </c>
       <c r="B3813" s="2" t="n">
-        <v>46061.70833333334</v>
+        <v>46062.70833333334</v>
       </c>
       <c r="C3813" t="n">
-        <v>111.91</v>
+        <v>169.06</v>
       </c>
     </row>
     <row r="3814">
       <c r="A3814" s="2" t="n">
-        <v>46061.67708333334</v>
+        <v>46062.67708333334</v>
       </c>
       <c r="B3814" s="2" t="n">
-        <v>46061.71875</v>
+        <v>46062.71875</v>
       </c>
       <c r="C3814" t="n">
-        <v>120.09</v>
+        <v>207.56</v>
       </c>
     </row>
     <row r="3815">
       <c r="A3815" s="2" t="n">
-        <v>46061.6875</v>
+        <v>46062.6875</v>
       </c>
       <c r="B3815" s="2" t="n">
-        <v>46061.72916666666</v>
+        <v>46062.72916666666</v>
       </c>
       <c r="C3815" t="n">
-        <v>125.41</v>
+        <v>216.59</v>
       </c>
     </row>
     <row r="3816">
       <c r="A3816" s="2" t="n">
-        <v>46061.69791666666</v>
+        <v>46062.69791666666</v>
       </c>
       <c r="B3816" s="2" t="n">
-        <v>46061.73958333334</v>
+        <v>46062.73958333334</v>
       </c>
       <c r="C3816" t="n">
-        <v>129.3</v>
+        <v>218.58</v>
       </c>
     </row>
     <row r="3817">
       <c r="A3817" s="2" t="n">
-        <v>46061.70833333334</v>
+        <v>46062.70833333334</v>
       </c>
       <c r="B3817" s="2" t="n">
-        <v>46061.75</v>
+        <v>46062.75</v>
       </c>
       <c r="C3817" t="n">
-        <v>126.95</v>
+        <v>181.73</v>
       </c>
     </row>
     <row r="3818">
       <c r="A3818" s="2" t="n">
-        <v>46061.71875</v>
+        <v>46062.71875</v>
       </c>
       <c r="B3818" s="2" t="n">
-        <v>46061.76041666666</v>
+        <v>46062.76041666666</v>
       </c>
       <c r="C3818" t="n">
-        <v>129.89</v>
+        <v>173.4</v>
       </c>
     </row>
     <row r="3819">
       <c r="A3819" s="2" t="n">
-        <v>46061.72916666666</v>
+        <v>46062.72916666666</v>
       </c>
       <c r="B3819" s="2" t="n">
-        <v>46061.77083333334</v>
+        <v>46062.77083333334</v>
       </c>
       <c r="C3819" t="n">
-        <v>132.55</v>
+        <v>165.84</v>
       </c>
     </row>
     <row r="3820">
       <c r="A3820" s="2" t="n">
-        <v>46061.73958333334</v>
+        <v>46062.73958333334</v>
       </c>
       <c r="B3820" s="2" t="n">
-        <v>46061.78125</v>
+        <v>46062.78125</v>
       </c>
       <c r="C3820" t="n">
-        <v>129.84</v>
+        <v>172.83</v>
       </c>
     </row>
     <row r="3821">
       <c r="A3821" s="2" t="n">
-        <v>46061.75</v>
+        <v>46062.75</v>
       </c>
       <c r="B3821" s="2" t="n">
-        <v>46061.79166666666</v>
+        <v>46062.79166666666</v>
       </c>
       <c r="C3821" t="n">
-        <v>132.96</v>
+        <v>183.64</v>
       </c>
     </row>
     <row r="3822">
       <c r="A3822" s="2" t="n">
-        <v>46061.76041666666</v>
+        <v>46062.76041666666</v>
       </c>
       <c r="B3822" s="2" t="n">
-        <v>46061.80208333334</v>
+        <v>46062.80208333334</v>
       </c>
       <c r="C3822" t="n">
-        <v>129.55</v>
+        <v>163.28</v>
       </c>
     </row>
     <row r="3823">
       <c r="A3823" s="2" t="n">
-        <v>46061.77083333334</v>
+        <v>46062.77083333334</v>
       </c>
       <c r="B3823" s="2" t="n">
-        <v>46061.8125</v>
+        <v>46062.8125</v>
       </c>
       <c r="C3823" t="n">
-        <v>125.09</v>
+        <v>152.48</v>
       </c>
     </row>
     <row r="3824">
       <c r="A3824" s="2" t="n">
-        <v>46061.78125</v>
+        <v>46062.78125</v>
       </c>
       <c r="B3824" s="2" t="n">
-        <v>46061.82291666666</v>
+        <v>46062.82291666666</v>
       </c>
       <c r="C3824" t="n">
-        <v>120</v>
+        <v>137.17</v>
       </c>
     </row>
     <row r="3825">
       <c r="A3825" s="2" t="n">
-        <v>46061.79166666666</v>
+        <v>46062.79166666666</v>
       </c>
       <c r="B3825" s="2" t="n">
-        <v>46061.83333333334</v>
+        <v>46062.83333333334</v>
       </c>
       <c r="C3825" t="n">
-        <v>122.21</v>
+        <v>153.8</v>
       </c>
     </row>
     <row r="3826">
       <c r="A3826" s="2" t="n">
-        <v>46061.80208333334</v>
+        <v>46062.80208333334</v>
       </c>
       <c r="B3826" s="2" t="n">
-        <v>46061.84375</v>
+        <v>46062.84375</v>
       </c>
       <c r="C3826" t="n">
-        <v>113.65</v>
+        <v>140.67</v>
       </c>
     </row>
     <row r="3827">
       <c r="A3827" s="2" t="n">
-        <v>46061.8125</v>
+        <v>46062.8125</v>
       </c>
       <c r="B3827" s="2" t="n">
-        <v>46061.85416666666</v>
+        <v>46062.85416666666</v>
       </c>
       <c r="C3827" t="n">
-        <v>109.35</v>
+        <v>132.99</v>
       </c>
     </row>
     <row r="3828">
       <c r="A3828" s="2" t="n">
-        <v>46061.82291666666</v>
+        <v>46062.82291666666</v>
       </c>
       <c r="B3828" s="2" t="n">
-        <v>46061.86458333334</v>
+        <v>46062.86458333334</v>
       </c>
       <c r="C3828" t="n">
-        <v>103.88</v>
+        <v>120.87</v>
       </c>
     </row>
     <row r="3829">
       <c r="A3829" s="2" t="n">
-        <v>46061.83333333334</v>
+        <v>46062.83333333334</v>
       </c>
       <c r="B3829" s="2" t="n">
-        <v>46061.875</v>
+        <v>46062.875</v>
       </c>
       <c r="C3829" t="n">
-        <v>109.68</v>
+        <v>139.22</v>
       </c>
     </row>
     <row r="3830">
       <c r="A3830" s="2" t="n">
-        <v>46061.84375</v>
+        <v>46062.84375</v>
       </c>
       <c r="B3830" s="2" t="n">
-        <v>46061.88541666666</v>
+        <v>46062.88541666666</v>
       </c>
       <c r="C3830" t="n">
-        <v>107.09</v>
+        <v>134.72</v>
       </c>
     </row>
     <row r="3831">
       <c r="A3831" s="2" t="n">
-        <v>46061.85416666666</v>
+        <v>46062.85416666666</v>
       </c>
       <c r="B3831" s="2" t="n">
-        <v>46061.89583333334</v>
+        <v>46062.89583333334</v>
       </c>
       <c r="C3831" t="n">
-        <v>103.63</v>
+        <v>122.19</v>
       </c>
     </row>
     <row r="3832">
       <c r="A3832" s="2" t="n">
-        <v>46061.86458333334</v>
+        <v>46062.86458333334</v>
       </c>
       <c r="B3832" s="2" t="n">
-        <v>46061.90625</v>
+        <v>46062.90625</v>
       </c>
       <c r="C3832" t="n">
-        <v>101.05</v>
+        <v>107.36</v>
       </c>
     </row>
     <row r="3833">
       <c r="A3833" s="2" t="n">
-        <v>46061.875</v>
+        <v>46062.875</v>
       </c>
       <c r="B3833" s="2" t="n">
-        <v>46061.91666666666</v>
+        <v>46062.91666666666</v>
       </c>
       <c r="C3833" t="n">
-        <v>105.51</v>
+        <v>120.93</v>
       </c>
     </row>
     <row r="3834">
       <c r="A3834" s="2" t="n">
-        <v>46061.88541666666</v>
+        <v>46062.88541666666</v>
       </c>
       <c r="B3834" s="2" t="n">
-        <v>46061.92708333334</v>
+        <v>46062.92708333334</v>
       </c>
       <c r="C3834" t="n">
-        <v>104.16</v>
+        <v>114.4</v>
       </c>
     </row>
     <row r="3835">
       <c r="A3835" s="2" t="n">
-        <v>46061.89583333334</v>
+        <v>46062.89583333334</v>
       </c>
       <c r="B3835" s="2" t="n">
-        <v>46061.9375</v>
+        <v>46062.9375</v>
       </c>
       <c r="C3835" t="n">
-        <v>104.14</v>
+        <v>118.43</v>
       </c>
     </row>
     <row r="3836">
       <c r="A3836" s="2" t="n">
-        <v>46061.90625</v>
+        <v>46062.90625</v>
       </c>
       <c r="B3836" s="2" t="n">
-        <v>46061.94791666666</v>
+        <v>46062.94791666666</v>
       </c>
       <c r="C3836" t="n">
-        <v>101.42</v>
+        <v>108.66</v>
       </c>
     </row>
     <row r="3837">
       <c r="A3837" s="2" t="n">
-        <v>46061.91666666666</v>
+        <v>46062.91666666666</v>
       </c>
       <c r="B3837" s="2" t="n">
-        <v>46061.95833333334</v>
+        <v>46062.95833333334</v>
       </c>
       <c r="C3837" t="n">
-        <v>102.25</v>
+        <v>110.85</v>
       </c>
     </row>
     <row r="3838">
       <c r="A3838" s="2" t="n">
-        <v>46061.92708333334</v>
+        <v>46062.92708333334</v>
       </c>
       <c r="B3838" s="2" t="n">
-        <v>46061.96875</v>
+        <v>46062.96875</v>
       </c>
       <c r="C3838" t="n">
-        <v>101.71</v>
+        <v>100.14</v>
       </c>
     </row>
     <row r="3839">
       <c r="A3839" s="2" t="n">
-        <v>46061.9375</v>
+        <v>46062.9375</v>
       </c>
       <c r="B3839" s="2" t="n">
-        <v>46061.97916666666</v>
+        <v>46062.97916666666</v>
       </c>
       <c r="C3839" t="n">
-        <v>100.28</v>
+        <v>102.34</v>
       </c>
     </row>
     <row r="3840">
       <c r="A3840" s="2" t="n">
-        <v>46061.94791666666</v>
+        <v>46062.94791666666</v>
       </c>
       <c r="B3840" s="2" t="n">
-        <v>46061.98958333334</v>
+        <v>46062.98958333334</v>
       </c>
       <c r="C3840" t="n">
-        <v>93.73999999999999</v>
+        <v>93.29000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update XLSX via API 09-02-2026, 14:38:42
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3840"/>
+  <dimension ref="A1:C3744"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41577,1062 +41577,6 @@
         <v>90.45999999999999</v>
       </c>
     </row>
-    <row r="3745">
-      <c r="A3745" s="2" t="n">
-        <v>46061.95833333334</v>
-      </c>
-      <c r="B3745" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="C3745" t="n">
-        <v>99.88</v>
-      </c>
-    </row>
-    <row r="3746">
-      <c r="A3746" s="2" t="n">
-        <v>46061.96875</v>
-      </c>
-      <c r="B3746" s="2" t="n">
-        <v>46062.01041666666</v>
-      </c>
-      <c r="C3746" t="n">
-        <v>97.3</v>
-      </c>
-    </row>
-    <row r="3747">
-      <c r="A3747" s="2" t="n">
-        <v>46061.97916666666</v>
-      </c>
-      <c r="B3747" s="2" t="n">
-        <v>46062.02083333334</v>
-      </c>
-      <c r="C3747" t="n">
-        <v>92.38</v>
-      </c>
-    </row>
-    <row r="3748">
-      <c r="A3748" s="2" t="n">
-        <v>46061.98958333334</v>
-      </c>
-      <c r="B3748" s="2" t="n">
-        <v>46062.03125</v>
-      </c>
-      <c r="C3748" t="n">
-        <v>89.40000000000001</v>
-      </c>
-    </row>
-    <row r="3749">
-      <c r="A3749" s="2" t="n">
-        <v>46062</v>
-      </c>
-      <c r="B3749" s="2" t="n">
-        <v>46062.04166666666</v>
-      </c>
-      <c r="C3749" t="n">
-        <v>95.92</v>
-      </c>
-    </row>
-    <row r="3750">
-      <c r="A3750" s="2" t="n">
-        <v>46062.01041666666</v>
-      </c>
-      <c r="B3750" s="2" t="n">
-        <v>46062.05208333334</v>
-      </c>
-      <c r="C3750" t="n">
-        <v>93.2</v>
-      </c>
-    </row>
-    <row r="3751">
-      <c r="A3751" s="2" t="n">
-        <v>46062.02083333334</v>
-      </c>
-      <c r="B3751" s="2" t="n">
-        <v>46062.0625</v>
-      </c>
-      <c r="C3751" t="n">
-        <v>92.94</v>
-      </c>
-    </row>
-    <row r="3752">
-      <c r="A3752" s="2" t="n">
-        <v>46062.03125</v>
-      </c>
-      <c r="B3752" s="2" t="n">
-        <v>46062.07291666666</v>
-      </c>
-      <c r="C3752" t="n">
-        <v>90.53</v>
-      </c>
-    </row>
-    <row r="3753">
-      <c r="A3753" s="2" t="n">
-        <v>46062.04166666666</v>
-      </c>
-      <c r="B3753" s="2" t="n">
-        <v>46062.08333333334</v>
-      </c>
-      <c r="C3753" t="n">
-        <v>94.06999999999999</v>
-      </c>
-    </row>
-    <row r="3754">
-      <c r="A3754" s="2" t="n">
-        <v>46062.05208333334</v>
-      </c>
-      <c r="B3754" s="2" t="n">
-        <v>46062.09375</v>
-      </c>
-      <c r="C3754" t="n">
-        <v>92.25</v>
-      </c>
-    </row>
-    <row r="3755">
-      <c r="A3755" s="2" t="n">
-        <v>46062.0625</v>
-      </c>
-      <c r="B3755" s="2" t="n">
-        <v>46062.10416666666</v>
-      </c>
-      <c r="C3755" t="n">
-        <v>92.75</v>
-      </c>
-    </row>
-    <row r="3756">
-      <c r="A3756" s="2" t="n">
-        <v>46062.07291666666</v>
-      </c>
-      <c r="B3756" s="2" t="n">
-        <v>46062.11458333334</v>
-      </c>
-      <c r="C3756" t="n">
-        <v>88.92</v>
-      </c>
-    </row>
-    <row r="3757">
-      <c r="A3757" s="2" t="n">
-        <v>46062.08333333334</v>
-      </c>
-      <c r="B3757" s="2" t="n">
-        <v>46062.125</v>
-      </c>
-      <c r="C3757" t="n">
-        <v>90.94</v>
-      </c>
-    </row>
-    <row r="3758">
-      <c r="A3758" s="2" t="n">
-        <v>46062.09375</v>
-      </c>
-      <c r="B3758" s="2" t="n">
-        <v>46062.13541666666</v>
-      </c>
-      <c r="C3758" t="n">
-        <v>90.03</v>
-      </c>
-    </row>
-    <row r="3759">
-      <c r="A3759" s="2" t="n">
-        <v>46062.10416666666</v>
-      </c>
-      <c r="B3759" s="2" t="n">
-        <v>46062.14583333334</v>
-      </c>
-      <c r="C3759" t="n">
-        <v>90.25</v>
-      </c>
-    </row>
-    <row r="3760">
-      <c r="A3760" s="2" t="n">
-        <v>46062.11458333334</v>
-      </c>
-      <c r="B3760" s="2" t="n">
-        <v>46062.15625</v>
-      </c>
-      <c r="C3760" t="n">
-        <v>89.77</v>
-      </c>
-    </row>
-    <row r="3761">
-      <c r="A3761" s="2" t="n">
-        <v>46062.125</v>
-      </c>
-      <c r="B3761" s="2" t="n">
-        <v>46062.16666666666</v>
-      </c>
-      <c r="C3761" t="n">
-        <v>87.87</v>
-      </c>
-    </row>
-    <row r="3762">
-      <c r="A3762" s="2" t="n">
-        <v>46062.13541666666</v>
-      </c>
-      <c r="B3762" s="2" t="n">
-        <v>46062.17708333334</v>
-      </c>
-      <c r="C3762" t="n">
-        <v>89.18000000000001</v>
-      </c>
-    </row>
-    <row r="3763">
-      <c r="A3763" s="2" t="n">
-        <v>46062.14583333334</v>
-      </c>
-      <c r="B3763" s="2" t="n">
-        <v>46062.1875</v>
-      </c>
-      <c r="C3763" t="n">
-        <v>90.11</v>
-      </c>
-    </row>
-    <row r="3764">
-      <c r="A3764" s="2" t="n">
-        <v>46062.15625</v>
-      </c>
-      <c r="B3764" s="2" t="n">
-        <v>46062.19791666666</v>
-      </c>
-      <c r="C3764" t="n">
-        <v>95.18000000000001</v>
-      </c>
-    </row>
-    <row r="3765">
-      <c r="A3765" s="2" t="n">
-        <v>46062.16666666666</v>
-      </c>
-      <c r="B3765" s="2" t="n">
-        <v>46062.20833333334</v>
-      </c>
-      <c r="C3765" t="n">
-        <v>91.87</v>
-      </c>
-    </row>
-    <row r="3766">
-      <c r="A3766" s="2" t="n">
-        <v>46062.17708333334</v>
-      </c>
-      <c r="B3766" s="2" t="n">
-        <v>46062.21875</v>
-      </c>
-      <c r="C3766" t="n">
-        <v>96.48</v>
-      </c>
-    </row>
-    <row r="3767">
-      <c r="A3767" s="2" t="n">
-        <v>46062.1875</v>
-      </c>
-      <c r="B3767" s="2" t="n">
-        <v>46062.22916666666</v>
-      </c>
-      <c r="C3767" t="n">
-        <v>101.27</v>
-      </c>
-    </row>
-    <row r="3768">
-      <c r="A3768" s="2" t="n">
-        <v>46062.19791666666</v>
-      </c>
-      <c r="B3768" s="2" t="n">
-        <v>46062.23958333334</v>
-      </c>
-      <c r="C3768" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3769">
-      <c r="A3769" s="2" t="n">
-        <v>46062.20833333334</v>
-      </c>
-      <c r="B3769" s="2" t="n">
-        <v>46062.25</v>
-      </c>
-      <c r="C3769" t="n">
-        <v>101.27</v>
-      </c>
-    </row>
-    <row r="3770">
-      <c r="A3770" s="2" t="n">
-        <v>46062.21875</v>
-      </c>
-      <c r="B3770" s="2" t="n">
-        <v>46062.26041666666</v>
-      </c>
-      <c r="C3770" t="n">
-        <v>116.41</v>
-      </c>
-    </row>
-    <row r="3771">
-      <c r="A3771" s="2" t="n">
-        <v>46062.22916666666</v>
-      </c>
-      <c r="B3771" s="2" t="n">
-        <v>46062.27083333334</v>
-      </c>
-      <c r="C3771" t="n">
-        <v>130.75</v>
-      </c>
-    </row>
-    <row r="3772">
-      <c r="A3772" s="2" t="n">
-        <v>46062.23958333334</v>
-      </c>
-      <c r="B3772" s="2" t="n">
-        <v>46062.28125</v>
-      </c>
-      <c r="C3772" t="n">
-        <v>158.33</v>
-      </c>
-    </row>
-    <row r="3773">
-      <c r="A3773" s="2" t="n">
-        <v>46062.25</v>
-      </c>
-      <c r="B3773" s="2" t="n">
-        <v>46062.29166666666</v>
-      </c>
-      <c r="C3773" t="n">
-        <v>129.99</v>
-      </c>
-    </row>
-    <row r="3774">
-      <c r="A3774" s="2" t="n">
-        <v>46062.26041666666</v>
-      </c>
-      <c r="B3774" s="2" t="n">
-        <v>46062.30208333334</v>
-      </c>
-      <c r="C3774" t="n">
-        <v>152.36</v>
-      </c>
-    </row>
-    <row r="3775">
-      <c r="A3775" s="2" t="n">
-        <v>46062.27083333334</v>
-      </c>
-      <c r="B3775" s="2" t="n">
-        <v>46062.3125</v>
-      </c>
-      <c r="C3775" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3776">
-      <c r="A3776" s="2" t="n">
-        <v>46062.28125</v>
-      </c>
-      <c r="B3776" s="2" t="n">
-        <v>46062.32291666666</v>
-      </c>
-      <c r="C3776" t="n">
-        <v>163.64</v>
-      </c>
-    </row>
-    <row r="3777">
-      <c r="A3777" s="2" t="n">
-        <v>46062.29166666666</v>
-      </c>
-      <c r="B3777" s="2" t="n">
-        <v>46062.33333333334</v>
-      </c>
-      <c r="C3777" t="n">
-        <v>170.29</v>
-      </c>
-    </row>
-    <row r="3778">
-      <c r="A3778" s="2" t="n">
-        <v>46062.30208333334</v>
-      </c>
-      <c r="B3778" s="2" t="n">
-        <v>46062.34375</v>
-      </c>
-      <c r="C3778" t="n">
-        <v>179.32</v>
-      </c>
-    </row>
-    <row r="3779">
-      <c r="A3779" s="2" t="n">
-        <v>46062.3125</v>
-      </c>
-      <c r="B3779" s="2" t="n">
-        <v>46062.35416666666</v>
-      </c>
-      <c r="C3779" t="n">
-        <v>179.34</v>
-      </c>
-    </row>
-    <row r="3780">
-      <c r="A3780" s="2" t="n">
-        <v>46062.32291666666</v>
-      </c>
-      <c r="B3780" s="2" t="n">
-        <v>46062.36458333334</v>
-      </c>
-      <c r="C3780" t="n">
-        <v>175.09</v>
-      </c>
-    </row>
-    <row r="3781">
-      <c r="A3781" s="2" t="n">
-        <v>46062.33333333334</v>
-      </c>
-      <c r="B3781" s="2" t="n">
-        <v>46062.375</v>
-      </c>
-      <c r="C3781" t="n">
-        <v>182.41</v>
-      </c>
-    </row>
-    <row r="3782">
-      <c r="A3782" s="2" t="n">
-        <v>46062.34375</v>
-      </c>
-      <c r="B3782" s="2" t="n">
-        <v>46062.38541666666</v>
-      </c>
-      <c r="C3782" t="n">
-        <v>171.32</v>
-      </c>
-    </row>
-    <row r="3783">
-      <c r="A3783" s="2" t="n">
-        <v>46062.35416666666</v>
-      </c>
-      <c r="B3783" s="2" t="n">
-        <v>46062.39583333334</v>
-      </c>
-      <c r="C3783" t="n">
-        <v>151.84</v>
-      </c>
-    </row>
-    <row r="3784">
-      <c r="A3784" s="2" t="n">
-        <v>46062.36458333334</v>
-      </c>
-      <c r="B3784" s="2" t="n">
-        <v>46062.40625</v>
-      </c>
-      <c r="C3784" t="n">
-        <v>148.06</v>
-      </c>
-    </row>
-    <row r="3785">
-      <c r="A3785" s="2" t="n">
-        <v>46062.375</v>
-      </c>
-      <c r="B3785" s="2" t="n">
-        <v>46062.41666666666</v>
-      </c>
-      <c r="C3785" t="n">
-        <v>158.59</v>
-      </c>
-    </row>
-    <row r="3786">
-      <c r="A3786" s="2" t="n">
-        <v>46062.38541666666</v>
-      </c>
-      <c r="B3786" s="2" t="n">
-        <v>46062.42708333334</v>
-      </c>
-      <c r="C3786" t="n">
-        <v>154.96</v>
-      </c>
-    </row>
-    <row r="3787">
-      <c r="A3787" s="2" t="n">
-        <v>46062.39583333334</v>
-      </c>
-      <c r="B3787" s="2" t="n">
-        <v>46062.4375</v>
-      </c>
-      <c r="C3787" t="n">
-        <v>146.04</v>
-      </c>
-    </row>
-    <row r="3788">
-      <c r="A3788" s="2" t="n">
-        <v>46062.40625</v>
-      </c>
-      <c r="B3788" s="2" t="n">
-        <v>46062.44791666666</v>
-      </c>
-      <c r="C3788" t="n">
-        <v>136.63</v>
-      </c>
-    </row>
-    <row r="3789">
-      <c r="A3789" s="2" t="n">
-        <v>46062.41666666666</v>
-      </c>
-      <c r="B3789" s="2" t="n">
-        <v>46062.45833333334</v>
-      </c>
-      <c r="C3789" t="n">
-        <v>142.94</v>
-      </c>
-    </row>
-    <row r="3790">
-      <c r="A3790" s="2" t="n">
-        <v>46062.42708333334</v>
-      </c>
-      <c r="B3790" s="2" t="n">
-        <v>46062.46875</v>
-      </c>
-      <c r="C3790" t="n">
-        <v>138.97</v>
-      </c>
-    </row>
-    <row r="3791">
-      <c r="A3791" s="2" t="n">
-        <v>46062.4375</v>
-      </c>
-      <c r="B3791" s="2" t="n">
-        <v>46062.47916666666</v>
-      </c>
-      <c r="C3791" t="n">
-        <v>136.31</v>
-      </c>
-    </row>
-    <row r="3792">
-      <c r="A3792" s="2" t="n">
-        <v>46062.44791666666</v>
-      </c>
-      <c r="B3792" s="2" t="n">
-        <v>46062.48958333334</v>
-      </c>
-      <c r="C3792" t="n">
-        <v>129.95</v>
-      </c>
-    </row>
-    <row r="3793">
-      <c r="A3793" s="2" t="n">
-        <v>46062.45833333334</v>
-      </c>
-      <c r="B3793" s="2" t="n">
-        <v>46062.5</v>
-      </c>
-      <c r="C3793" t="n">
-        <v>138.44</v>
-      </c>
-    </row>
-    <row r="3794">
-      <c r="A3794" s="2" t="n">
-        <v>46062.46875</v>
-      </c>
-      <c r="B3794" s="2" t="n">
-        <v>46062.51041666666</v>
-      </c>
-      <c r="C3794" t="n">
-        <v>131.46</v>
-      </c>
-    </row>
-    <row r="3795">
-      <c r="A3795" s="2" t="n">
-        <v>46062.47916666666</v>
-      </c>
-      <c r="B3795" s="2" t="n">
-        <v>46062.52083333334</v>
-      </c>
-      <c r="C3795" t="n">
-        <v>129.11</v>
-      </c>
-    </row>
-    <row r="3796">
-      <c r="A3796" s="2" t="n">
-        <v>46062.48958333334</v>
-      </c>
-      <c r="B3796" s="2" t="n">
-        <v>46062.53125</v>
-      </c>
-      <c r="C3796" t="n">
-        <v>122.74</v>
-      </c>
-    </row>
-    <row r="3797">
-      <c r="A3797" s="2" t="n">
-        <v>46062.5</v>
-      </c>
-      <c r="B3797" s="2" t="n">
-        <v>46062.54166666666</v>
-      </c>
-      <c r="C3797" t="n">
-        <v>130.01</v>
-      </c>
-    </row>
-    <row r="3798">
-      <c r="A3798" s="2" t="n">
-        <v>46062.51041666666</v>
-      </c>
-      <c r="B3798" s="2" t="n">
-        <v>46062.55208333334</v>
-      </c>
-      <c r="C3798" t="n">
-        <v>128.36</v>
-      </c>
-    </row>
-    <row r="3799">
-      <c r="A3799" s="2" t="n">
-        <v>46062.52083333334</v>
-      </c>
-      <c r="B3799" s="2" t="n">
-        <v>46062.5625</v>
-      </c>
-      <c r="C3799" t="n">
-        <v>124.6</v>
-      </c>
-    </row>
-    <row r="3800">
-      <c r="A3800" s="2" t="n">
-        <v>46062.53125</v>
-      </c>
-      <c r="B3800" s="2" t="n">
-        <v>46062.57291666666</v>
-      </c>
-      <c r="C3800" t="n">
-        <v>120.26</v>
-      </c>
-    </row>
-    <row r="3801">
-      <c r="A3801" s="2" t="n">
-        <v>46062.54166666666</v>
-      </c>
-      <c r="B3801" s="2" t="n">
-        <v>46062.58333333334</v>
-      </c>
-      <c r="C3801" t="n">
-        <v>116.47</v>
-      </c>
-    </row>
-    <row r="3802">
-      <c r="A3802" s="2" t="n">
-        <v>46062.55208333334</v>
-      </c>
-      <c r="B3802" s="2" t="n">
-        <v>46062.59375</v>
-      </c>
-      <c r="C3802" t="n">
-        <v>125.23</v>
-      </c>
-    </row>
-    <row r="3803">
-      <c r="A3803" s="2" t="n">
-        <v>46062.5625</v>
-      </c>
-      <c r="B3803" s="2" t="n">
-        <v>46062.60416666666</v>
-      </c>
-      <c r="C3803" t="n">
-        <v>132.18</v>
-      </c>
-    </row>
-    <row r="3804">
-      <c r="A3804" s="2" t="n">
-        <v>46062.57291666666</v>
-      </c>
-      <c r="B3804" s="2" t="n">
-        <v>46062.61458333334</v>
-      </c>
-      <c r="C3804" t="n">
-        <v>140.5</v>
-      </c>
-    </row>
-    <row r="3805">
-      <c r="A3805" s="2" t="n">
-        <v>46062.58333333334</v>
-      </c>
-      <c r="B3805" s="2" t="n">
-        <v>46062.625</v>
-      </c>
-      <c r="C3805" t="n">
-        <v>120.08</v>
-      </c>
-    </row>
-    <row r="3806">
-      <c r="A3806" s="2" t="n">
-        <v>46062.59375</v>
-      </c>
-      <c r="B3806" s="2" t="n">
-        <v>46062.63541666666</v>
-      </c>
-      <c r="C3806" t="n">
-        <v>129.9</v>
-      </c>
-    </row>
-    <row r="3807">
-      <c r="A3807" s="2" t="n">
-        <v>46062.60416666666</v>
-      </c>
-      <c r="B3807" s="2" t="n">
-        <v>46062.64583333334</v>
-      </c>
-      <c r="C3807" t="n">
-        <v>145.32</v>
-      </c>
-    </row>
-    <row r="3808">
-      <c r="A3808" s="2" t="n">
-        <v>46062.61458333334</v>
-      </c>
-      <c r="B3808" s="2" t="n">
-        <v>46062.65625</v>
-      </c>
-      <c r="C3808" t="n">
-        <v>157.91</v>
-      </c>
-    </row>
-    <row r="3809">
-      <c r="A3809" s="2" t="n">
-        <v>46062.625</v>
-      </c>
-      <c r="B3809" s="2" t="n">
-        <v>46062.66666666666</v>
-      </c>
-      <c r="C3809" t="n">
-        <v>128.61</v>
-      </c>
-    </row>
-    <row r="3810">
-      <c r="A3810" s="2" t="n">
-        <v>46062.63541666666</v>
-      </c>
-      <c r="B3810" s="2" t="n">
-        <v>46062.67708333334</v>
-      </c>
-      <c r="C3810" t="n">
-        <v>148.24</v>
-      </c>
-    </row>
-    <row r="3811">
-      <c r="A3811" s="2" t="n">
-        <v>46062.64583333334</v>
-      </c>
-      <c r="B3811" s="2" t="n">
-        <v>46062.6875</v>
-      </c>
-      <c r="C3811" t="n">
-        <v>168.24</v>
-      </c>
-    </row>
-    <row r="3812">
-      <c r="A3812" s="2" t="n">
-        <v>46062.65625</v>
-      </c>
-      <c r="B3812" s="2" t="n">
-        <v>46062.69791666666</v>
-      </c>
-      <c r="C3812" t="n">
-        <v>175.4</v>
-      </c>
-    </row>
-    <row r="3813">
-      <c r="A3813" s="2" t="n">
-        <v>46062.66666666666</v>
-      </c>
-      <c r="B3813" s="2" t="n">
-        <v>46062.70833333334</v>
-      </c>
-      <c r="C3813" t="n">
-        <v>169.06</v>
-      </c>
-    </row>
-    <row r="3814">
-      <c r="A3814" s="2" t="n">
-        <v>46062.67708333334</v>
-      </c>
-      <c r="B3814" s="2" t="n">
-        <v>46062.71875</v>
-      </c>
-      <c r="C3814" t="n">
-        <v>207.56</v>
-      </c>
-    </row>
-    <row r="3815">
-      <c r="A3815" s="2" t="n">
-        <v>46062.6875</v>
-      </c>
-      <c r="B3815" s="2" t="n">
-        <v>46062.72916666666</v>
-      </c>
-      <c r="C3815" t="n">
-        <v>216.59</v>
-      </c>
-    </row>
-    <row r="3816">
-      <c r="A3816" s="2" t="n">
-        <v>46062.69791666666</v>
-      </c>
-      <c r="B3816" s="2" t="n">
-        <v>46062.73958333334</v>
-      </c>
-      <c r="C3816" t="n">
-        <v>218.58</v>
-      </c>
-    </row>
-    <row r="3817">
-      <c r="A3817" s="2" t="n">
-        <v>46062.70833333334</v>
-      </c>
-      <c r="B3817" s="2" t="n">
-        <v>46062.75</v>
-      </c>
-      <c r="C3817" t="n">
-        <v>181.73</v>
-      </c>
-    </row>
-    <row r="3818">
-      <c r="A3818" s="2" t="n">
-        <v>46062.71875</v>
-      </c>
-      <c r="B3818" s="2" t="n">
-        <v>46062.76041666666</v>
-      </c>
-      <c r="C3818" t="n">
-        <v>173.4</v>
-      </c>
-    </row>
-    <row r="3819">
-      <c r="A3819" s="2" t="n">
-        <v>46062.72916666666</v>
-      </c>
-      <c r="B3819" s="2" t="n">
-        <v>46062.77083333334</v>
-      </c>
-      <c r="C3819" t="n">
-        <v>165.84</v>
-      </c>
-    </row>
-    <row r="3820">
-      <c r="A3820" s="2" t="n">
-        <v>46062.73958333334</v>
-      </c>
-      <c r="B3820" s="2" t="n">
-        <v>46062.78125</v>
-      </c>
-      <c r="C3820" t="n">
-        <v>172.83</v>
-      </c>
-    </row>
-    <row r="3821">
-      <c r="A3821" s="2" t="n">
-        <v>46062.75</v>
-      </c>
-      <c r="B3821" s="2" t="n">
-        <v>46062.79166666666</v>
-      </c>
-      <c r="C3821" t="n">
-        <v>183.64</v>
-      </c>
-    </row>
-    <row r="3822">
-      <c r="A3822" s="2" t="n">
-        <v>46062.76041666666</v>
-      </c>
-      <c r="B3822" s="2" t="n">
-        <v>46062.80208333334</v>
-      </c>
-      <c r="C3822" t="n">
-        <v>163.28</v>
-      </c>
-    </row>
-    <row r="3823">
-      <c r="A3823" s="2" t="n">
-        <v>46062.77083333334</v>
-      </c>
-      <c r="B3823" s="2" t="n">
-        <v>46062.8125</v>
-      </c>
-      <c r="C3823" t="n">
-        <v>152.48</v>
-      </c>
-    </row>
-    <row r="3824">
-      <c r="A3824" s="2" t="n">
-        <v>46062.78125</v>
-      </c>
-      <c r="B3824" s="2" t="n">
-        <v>46062.82291666666</v>
-      </c>
-      <c r="C3824" t="n">
-        <v>137.17</v>
-      </c>
-    </row>
-    <row r="3825">
-      <c r="A3825" s="2" t="n">
-        <v>46062.79166666666</v>
-      </c>
-      <c r="B3825" s="2" t="n">
-        <v>46062.83333333334</v>
-      </c>
-      <c r="C3825" t="n">
-        <v>153.8</v>
-      </c>
-    </row>
-    <row r="3826">
-      <c r="A3826" s="2" t="n">
-        <v>46062.80208333334</v>
-      </c>
-      <c r="B3826" s="2" t="n">
-        <v>46062.84375</v>
-      </c>
-      <c r="C3826" t="n">
-        <v>140.67</v>
-      </c>
-    </row>
-    <row r="3827">
-      <c r="A3827" s="2" t="n">
-        <v>46062.8125</v>
-      </c>
-      <c r="B3827" s="2" t="n">
-        <v>46062.85416666666</v>
-      </c>
-      <c r="C3827" t="n">
-        <v>132.99</v>
-      </c>
-    </row>
-    <row r="3828">
-      <c r="A3828" s="2" t="n">
-        <v>46062.82291666666</v>
-      </c>
-      <c r="B3828" s="2" t="n">
-        <v>46062.86458333334</v>
-      </c>
-      <c r="C3828" t="n">
-        <v>120.87</v>
-      </c>
-    </row>
-    <row r="3829">
-      <c r="A3829" s="2" t="n">
-        <v>46062.83333333334</v>
-      </c>
-      <c r="B3829" s="2" t="n">
-        <v>46062.875</v>
-      </c>
-      <c r="C3829" t="n">
-        <v>139.22</v>
-      </c>
-    </row>
-    <row r="3830">
-      <c r="A3830" s="2" t="n">
-        <v>46062.84375</v>
-      </c>
-      <c r="B3830" s="2" t="n">
-        <v>46062.88541666666</v>
-      </c>
-      <c r="C3830" t="n">
-        <v>134.72</v>
-      </c>
-    </row>
-    <row r="3831">
-      <c r="A3831" s="2" t="n">
-        <v>46062.85416666666</v>
-      </c>
-      <c r="B3831" s="2" t="n">
-        <v>46062.89583333334</v>
-      </c>
-      <c r="C3831" t="n">
-        <v>122.19</v>
-      </c>
-    </row>
-    <row r="3832">
-      <c r="A3832" s="2" t="n">
-        <v>46062.86458333334</v>
-      </c>
-      <c r="B3832" s="2" t="n">
-        <v>46062.90625</v>
-      </c>
-      <c r="C3832" t="n">
-        <v>107.36</v>
-      </c>
-    </row>
-    <row r="3833">
-      <c r="A3833" s="2" t="n">
-        <v>46062.875</v>
-      </c>
-      <c r="B3833" s="2" t="n">
-        <v>46062.91666666666</v>
-      </c>
-      <c r="C3833" t="n">
-        <v>120.93</v>
-      </c>
-    </row>
-    <row r="3834">
-      <c r="A3834" s="2" t="n">
-        <v>46062.88541666666</v>
-      </c>
-      <c r="B3834" s="2" t="n">
-        <v>46062.92708333334</v>
-      </c>
-      <c r="C3834" t="n">
-        <v>114.4</v>
-      </c>
-    </row>
-    <row r="3835">
-      <c r="A3835" s="2" t="n">
-        <v>46062.89583333334</v>
-      </c>
-      <c r="B3835" s="2" t="n">
-        <v>46062.9375</v>
-      </c>
-      <c r="C3835" t="n">
-        <v>118.43</v>
-      </c>
-    </row>
-    <row r="3836">
-      <c r="A3836" s="2" t="n">
-        <v>46062.90625</v>
-      </c>
-      <c r="B3836" s="2" t="n">
-        <v>46062.94791666666</v>
-      </c>
-      <c r="C3836" t="n">
-        <v>108.66</v>
-      </c>
-    </row>
-    <row r="3837">
-      <c r="A3837" s="2" t="n">
-        <v>46062.91666666666</v>
-      </c>
-      <c r="B3837" s="2" t="n">
-        <v>46062.95833333334</v>
-      </c>
-      <c r="C3837" t="n">
-        <v>110.85</v>
-      </c>
-    </row>
-    <row r="3838">
-      <c r="A3838" s="2" t="n">
-        <v>46062.92708333334</v>
-      </c>
-      <c r="B3838" s="2" t="n">
-        <v>46062.96875</v>
-      </c>
-      <c r="C3838" t="n">
-        <v>100.14</v>
-      </c>
-    </row>
-    <row r="3839">
-      <c r="A3839" s="2" t="n">
-        <v>46062.9375</v>
-      </c>
-      <c r="B3839" s="2" t="n">
-        <v>46062.97916666666</v>
-      </c>
-      <c r="C3839" t="n">
-        <v>102.34</v>
-      </c>
-    </row>
-    <row r="3840">
-      <c r="A3840" s="2" t="n">
-        <v>46062.94791666666</v>
-      </c>
-      <c r="B3840" s="2" t="n">
-        <v>46062.98958333334</v>
-      </c>
-      <c r="C3840" t="n">
-        <v>93.29000000000001</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update XLSX via API 09-02-2026, 14:27:10
</commit_message>
<xml_diff>
--- a/day_ahead_prices.xlsx
+++ b/day_ahead_prices.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>